<commit_message>
Convert memberId to number for backend API compatibility
</commit_message>
<xml_diff>
--- a/members .xlsx
+++ b/members .xlsx
@@ -3,17 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{6CB9A2B6-4F01-4B41-9A3D-F0FCC10938AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8928E5EC-7462-4CA7-9430-461AD5A1DD26}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{B7497AC0-A7B1-4A41-910A-4EC7CFA4F027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7B1937D-6B92-4F47-A78F-85135F12C706}"/>
   <bookViews>
-    <workbookView xWindow="43905" yWindow="2325" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -29,8 +32,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="221">
   <si>
     <t>HORIZON-HOUSE MASTER LIST</t>
   </si>
@@ -624,9 +649,6 @@
     <t>liz@horizon-house.org</t>
   </si>
   <si>
-    <t>0141</t>
-  </si>
-  <si>
     <t>HORIZON HOUSE SOBER LIVING DAILY CENSUS</t>
   </si>
   <si>
@@ -729,19 +751,7 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Barney</t>
-  </si>
-  <si>
-    <t>Rubble</t>
-  </si>
-  <si>
-    <t>Wilma</t>
-  </si>
-  <si>
-    <t>Flintstone</t>
+    <t>0802</t>
   </si>
 </sst>
 </file>
@@ -993,12 +1003,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFD739E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1045,6 +1049,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD739E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -1579,28 +1589,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1647,12 +1645,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1664,57 +1662,57 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="23" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1733,24 +1731,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="19" fillId="12" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="19" fillId="11" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1766,37 +1776,76 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1808,56 +1857,26 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1868,16 +1887,7 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2354,6 +2364,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFD739E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2363,10 +2378,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2688,34 +2699,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1796875" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="12" width="6.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.54296875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.54296875" customWidth="1"/>
-    <col min="15" max="15" width="8.7265625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="6.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="10.81640625" customWidth="1"/>
-    <col min="18" max="18" width="7.453125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" customWidth="1"/>
-    <col min="20" max="20" width="23.7265625" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="136" t="s">
         <v>0</v>
@@ -2739,7 +2750,7 @@
       <c r="S1" s="136"/>
       <c r="T1" s="136"/>
     </row>
-    <row r="2" spans="1:22" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="137" t="s">
         <v>1</v>
       </c>
@@ -2748,7 +2759,7 @@
       <c r="E2" s="137"/>
       <c r="F2" s="138">
         <f ca="1">(TODAY())</f>
-        <v>46059</v>
+        <v>46061</v>
       </c>
       <c r="G2" s="138"/>
       <c r="H2" s="3"/>
@@ -2758,7 +2769,7 @@
       </c>
       <c r="K2" s="5">
         <f>O2+Q2</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
@@ -2767,14 +2778,14 @@
       </c>
       <c r="O2" s="8">
         <f>COUNTIF(E5:E202,"M")</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="10">
         <f>COUNTIF(E5:E202,"F")</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>5</v>
@@ -2783,7 +2794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="139" t="s">
         <v>7</v>
       </c>
@@ -2804,7 +2815,7 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="1:22" s="12" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" s="12" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -2872,7 +2883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2900,7 +2911,7 @@
       </c>
       <c r="J5" s="25">
         <f ca="1">(TODAY()-H5)</f>
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>33</v>
@@ -2924,7 +2935,7 @@
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
     </row>
-    <row r="6" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>A5+1</f>
         <v>2</v>
@@ -2979,12 +2990,12 @@
       </c>
       <c r="R6" s="31">
         <f ca="1">IF(Q6="","",(TODAY()-Q6))</f>
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A70" si="0">A6+1</f>
         <v>3</v>
@@ -3036,7 +3047,7 @@
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3088,7 +3099,7 @@
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3141,14 +3152,14 @@
       </c>
       <c r="R9" s="31">
         <f ca="1">IF(Q9="","",(TODAY()-Q9))</f>
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="S9" s="23"/>
       <c r="T9" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3203,12 +3214,12 @@
       </c>
       <c r="R10" s="31">
         <f t="shared" ref="R10:R33" ca="1" si="4">IF(Q10="","",(TODAY()-Q10))</f>
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3266,7 +3277,7 @@
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
     </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3319,7 +3330,7 @@
       <c r="S12" s="23"/>
       <c r="T12" s="23"/>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3372,12 +3383,12 @@
       </c>
       <c r="R13" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
     </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3430,12 +3441,12 @@
       </c>
       <c r="R14" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3488,14 +3499,14 @@
       </c>
       <c r="R15" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="S15" s="23" t="s">
         <v>65</v>
       </c>
       <c r="T15" s="23"/>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3548,14 +3559,14 @@
       </c>
       <c r="R16" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="S16" s="23" t="s">
         <v>70</v>
       </c>
       <c r="T16" s="23"/>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3607,7 +3618,7 @@
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3659,7 +3670,7 @@
       <c r="S18" s="23"/>
       <c r="T18" s="23"/>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3712,14 +3723,14 @@
       </c>
       <c r="R19" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="S19" s="23" t="s">
         <v>79</v>
       </c>
       <c r="T19" s="23"/>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3749,7 +3760,7 @@
       <c r="I20" s="39"/>
       <c r="J20" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="K20" s="41" t="s">
         <v>50</v>
@@ -3770,14 +3781,14 @@
       </c>
       <c r="R20" s="41">
         <f t="shared" ca="1" si="4"/>
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="S20" s="39" t="s">
         <v>84</v>
       </c>
       <c r="T20" s="39"/>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3828,12 +3839,12 @@
       </c>
       <c r="R21" s="25">
         <f t="shared" ca="1" si="4"/>
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3885,12 +3896,12 @@
       </c>
       <c r="R22" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3944,14 +3955,14 @@
       </c>
       <c r="R23" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="S23" s="23"/>
       <c r="T23" s="46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4001,7 +4012,7 @@
       </c>
       <c r="R24" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="S24" s="23" t="s">
         <v>99</v>
@@ -4010,7 +4021,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4060,7 +4071,7 @@
       </c>
       <c r="R25" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="S25" s="23" t="s">
         <v>103</v>
@@ -4069,7 +4080,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4119,14 +4130,14 @@
       </c>
       <c r="R26" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="S26" s="23"/>
       <c r="T26" s="46" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4176,14 +4187,14 @@
       </c>
       <c r="R27" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="S27" s="23"/>
       <c r="T27" s="46" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4233,7 +4244,7 @@
       </c>
       <c r="R28" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="S28" s="23">
         <v>4066655983</v>
@@ -4242,7 +4253,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4294,12 +4305,12 @@
       </c>
       <c r="R29" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="S29" s="23"/>
       <c r="T29" s="23"/>
     </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4351,7 +4362,7 @@
       </c>
       <c r="R30" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="S30" s="23" t="s">
         <v>119</v>
@@ -4363,7 +4374,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4417,7 +4428,7 @@
       </c>
       <c r="R31" s="31">
         <f t="shared" ref="R31" ca="1" si="7">IF(Q31="","",(TODAY()-Q31))</f>
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="S31" s="23" t="s">
         <v>126</v>
@@ -4426,7 +4437,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4476,14 +4487,14 @@
       </c>
       <c r="R32" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="S32" s="23"/>
       <c r="T32" s="46" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4537,14 +4548,14 @@
       </c>
       <c r="R33" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="S33" s="23"/>
       <c r="T33" s="46" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4598,7 +4609,7 @@
       </c>
       <c r="R34" s="31">
         <f t="shared" ref="R34:R39" ca="1" si="9">IF(Q34="","",(TODAY()-Q34))</f>
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="S34" s="23" t="s">
         <v>139</v>
@@ -4607,7 +4618,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4661,14 +4672,14 @@
       </c>
       <c r="R35" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="S35" s="23"/>
       <c r="T35" s="46" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4722,7 +4733,7 @@
       </c>
       <c r="R36" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="S36" s="23" t="s">
         <v>148</v>
@@ -4731,7 +4742,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4785,7 +4796,7 @@
       </c>
       <c r="R37" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="S37" s="23" t="s">
         <v>153</v>
@@ -4794,7 +4805,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4848,14 +4859,14 @@
       </c>
       <c r="R38" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="S38" s="23" t="s">
         <v>157</v>
       </c>
       <c r="T38" s="23"/>
     </row>
-    <row r="39" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4909,14 +4920,14 @@
       </c>
       <c r="R39" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S39" s="23" t="s">
         <v>162</v>
       </c>
       <c r="T39" s="23"/>
     </row>
-    <row r="40" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4968,7 +4979,7 @@
       </c>
       <c r="R40" s="31">
         <f ca="1">IF(Q40="","",(TODAY()-Q40))</f>
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="S40" s="50" t="s">
         <v>165</v>
@@ -4980,133 +4991,133 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="53">
+      <c r="C41" s="130">
         <v>137</v>
       </c>
-      <c r="D41" s="54">
+      <c r="D41" s="131">
         <v>3</v>
       </c>
-      <c r="E41" s="52" t="s">
+      <c r="E41" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="F41" s="52" t="s">
+      <c r="F41" s="129" t="s">
         <v>167</v>
       </c>
-      <c r="G41" s="52" t="s">
+      <c r="G41" s="129" t="s">
         <v>168</v>
       </c>
-      <c r="H41" s="55">
+      <c r="H41" s="132">
         <v>45936</v>
       </c>
-      <c r="I41" s="55">
+      <c r="I41" s="132">
         <v>46033</v>
       </c>
-      <c r="J41" s="54">
+      <c r="J41" s="131">
         <f t="shared" ref="J41:J44" ca="1" si="10">IF(H41="","",IF(I41="",TODAY()-H41,DATEDIF(H41,I41,"d")))</f>
         <v>97</v>
       </c>
-      <c r="K41" s="54" t="s">
+      <c r="K41" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="L41" s="56"/>
-      <c r="M41" s="54" t="s">
+      <c r="L41" s="133"/>
+      <c r="M41" s="131" t="s">
         <v>138</v>
       </c>
-      <c r="N41" s="52">
+      <c r="N41" s="129">
         <v>1500</v>
       </c>
-      <c r="O41" s="54"/>
-      <c r="P41" s="55">
+      <c r="O41" s="131"/>
+      <c r="P41" s="132">
         <v>34191</v>
       </c>
-      <c r="Q41" s="55">
+      <c r="Q41" s="132">
         <v>45941</v>
       </c>
-      <c r="R41" s="54">
+      <c r="R41" s="131">
         <f t="shared" ref="R41:R50" ca="1" si="11">IF(Q41="","",(TODAY()-Q41))</f>
-        <v>118</v>
-      </c>
-      <c r="S41" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="S41" s="129" t="s">
         <v>169</v>
       </c>
-      <c r="T41" s="57" t="s">
+      <c r="T41" s="134" t="s">
         <v>170</v>
       </c>
       <c r="V41" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="53">
+      <c r="C42" s="130">
         <v>138</v>
       </c>
-      <c r="D42" s="54">
+      <c r="D42" s="131">
         <v>2</v>
       </c>
-      <c r="E42" s="52" t="s">
+      <c r="E42" s="129" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="52" t="s">
+      <c r="F42" s="129" t="s">
         <v>172</v>
       </c>
-      <c r="G42" s="52" t="s">
+      <c r="G42" s="129" t="s">
         <v>173</v>
       </c>
-      <c r="H42" s="55">
+      <c r="H42" s="132">
         <v>45954</v>
       </c>
-      <c r="I42" s="55">
+      <c r="I42" s="132">
         <v>46058</v>
       </c>
-      <c r="J42" s="54">
+      <c r="J42" s="131">
         <f t="shared" ca="1" si="10"/>
         <v>104</v>
       </c>
-      <c r="K42" s="54" t="s">
+      <c r="K42" s="131" t="s">
         <v>75</v>
       </c>
-      <c r="L42" s="56"/>
-      <c r="M42" s="54" t="s">
+      <c r="L42" s="133"/>
+      <c r="M42" s="131" t="s">
         <v>138</v>
       </c>
-      <c r="N42" s="52">
+      <c r="N42" s="129">
         <v>1500</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="55">
+      <c r="O42" s="131"/>
+      <c r="P42" s="132">
         <v>30045</v>
       </c>
-      <c r="Q42" s="55">
+      <c r="Q42" s="132">
         <v>45860</v>
       </c>
-      <c r="R42" s="54">
+      <c r="R42" s="131">
         <f t="shared" ca="1" si="11"/>
-        <v>199</v>
-      </c>
-      <c r="S42" s="52"/>
-      <c r="T42" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="S42" s="129"/>
+      <c r="T42" s="134" t="s">
         <v>174</v>
       </c>
       <c r="U42">
         <v>1222</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5135,7 +5146,7 @@
       <c r="I43" s="42"/>
       <c r="J43" s="41">
         <f t="shared" ca="1" si="10"/>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K43" s="41" t="s">
         <v>39</v>
@@ -5158,7 +5169,7 @@
       </c>
       <c r="R43" s="41">
         <f t="shared" ca="1" si="11"/>
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S43" s="39" t="s">
         <v>162</v>
@@ -5168,7 +5179,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -5197,7 +5208,7 @@
       <c r="I44" s="39"/>
       <c r="J44" s="41">
         <f t="shared" ca="1" si="10"/>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K44" s="41" t="s">
         <v>42</v>
@@ -5210,19 +5221,23 @@
         <v>1200</v>
       </c>
       <c r="O44" s="41"/>
-      <c r="P44" s="42"/>
-      <c r="Q44" s="42"/>
-      <c r="R44" s="41" t="str">
+      <c r="P44" s="42">
+        <v>36740</v>
+      </c>
+      <c r="Q44" s="42">
+        <v>45962</v>
+      </c>
+      <c r="R44" s="41">
         <f t="shared" ca="1" si="11"/>
-        <v/>
+        <v>99</v>
       </c>
       <c r="S44" s="39"/>
       <c r="T44" s="39"/>
-      <c r="U44">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U44" s="135" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -5230,44 +5245,19 @@
       <c r="B45" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="58">
-        <v>141</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>221</v>
-      </c>
-      <c r="F45" t="s">
-        <v>222</v>
-      </c>
-      <c r="G45" t="s">
-        <v>223</v>
-      </c>
-      <c r="H45" s="135">
-        <v>46058</v>
-      </c>
-      <c r="L45" s="59"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="1"/>
+      <c r="L45" s="53"/>
       <c r="N45">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P45" s="135">
-        <v>36560</v>
-      </c>
-      <c r="Q45" s="135">
-        <v>45995</v>
-      </c>
-      <c r="R45" s="1">
+      <c r="R45" s="1" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>64</v>
-      </c>
-      <c r="U45">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -5275,44 +5265,23 @@
       <c r="B46" t="s">
         <v>176</v>
       </c>
-      <c r="C46" s="58">
-        <v>142</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>31</v>
-      </c>
-      <c r="F46" t="s">
-        <v>224</v>
-      </c>
-      <c r="G46" t="s">
-        <v>225</v>
-      </c>
-      <c r="H46" s="135">
-        <v>46058</v>
-      </c>
-      <c r="L46" s="59"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="1"/>
+      <c r="L46" s="53"/>
       <c r="N46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P46" s="135">
-        <v>35471</v>
-      </c>
-      <c r="Q46" s="135">
-        <v>46001</v>
-      </c>
-      <c r="R46" s="1">
+      <c r="R46" s="1" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>58</v>
-      </c>
-      <c r="U46">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v/>
+      </c>
+      <c r="T46" cm="1">
+        <f t="array" aca="1" ref="T46" ca="1">+A46:F46:T47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -5320,9 +5289,9 @@
       <c r="B47" t="s">
         <v>176</v>
       </c>
-      <c r="C47" s="58"/>
+      <c r="C47" s="52"/>
       <c r="D47" s="1"/>
-      <c r="L47" s="59"/>
+      <c r="L47" s="53"/>
       <c r="N47">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5332,7 +5301,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -5340,9 +5309,9 @@
       <c r="B48" t="s">
         <v>176</v>
       </c>
-      <c r="C48" s="58"/>
+      <c r="C48" s="52"/>
       <c r="D48" s="1"/>
-      <c r="L48" s="59"/>
+      <c r="L48" s="53"/>
       <c r="N48">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5352,7 +5321,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5360,9 +5329,9 @@
       <c r="B49" t="s">
         <v>176</v>
       </c>
-      <c r="C49" s="58"/>
+      <c r="C49" s="52"/>
       <c r="D49" s="1"/>
-      <c r="L49" s="59"/>
+      <c r="L49" s="53"/>
       <c r="N49">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5372,7 +5341,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -5380,9 +5349,9 @@
       <c r="B50" t="s">
         <v>176</v>
       </c>
-      <c r="C50" s="58"/>
+      <c r="C50" s="52"/>
       <c r="D50" s="1"/>
-      <c r="L50" s="59"/>
+      <c r="L50" s="53"/>
       <c r="N50">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -5392,7 +5361,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5400,15 +5369,15 @@
       <c r="B51" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="58"/>
+      <c r="C51" s="52"/>
       <c r="D51" s="1"/>
-      <c r="L51" s="59"/>
+      <c r="L51" s="53"/>
       <c r="N51">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5416,15 +5385,15 @@
       <c r="B52" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="58"/>
+      <c r="C52" s="52"/>
       <c r="D52" s="1"/>
-      <c r="L52" s="59"/>
+      <c r="L52" s="53"/>
       <c r="N52">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -5432,15 +5401,15 @@
       <c r="B53" t="s">
         <v>176</v>
       </c>
-      <c r="C53" s="58"/>
+      <c r="C53" s="52"/>
       <c r="D53" s="1"/>
-      <c r="L53" s="59"/>
+      <c r="L53" s="53"/>
       <c r="N53">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -5448,15 +5417,15 @@
       <c r="B54" t="s">
         <v>176</v>
       </c>
-      <c r="C54" s="58"/>
+      <c r="C54" s="52"/>
       <c r="D54" s="1"/>
-      <c r="L54" s="59"/>
+      <c r="L54" s="53"/>
       <c r="N54">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -5464,15 +5433,15 @@
       <c r="B55" t="s">
         <v>176</v>
       </c>
-      <c r="C55" s="58"/>
+      <c r="C55" s="52"/>
       <c r="D55" s="1"/>
-      <c r="L55" s="59"/>
+      <c r="L55" s="53"/>
       <c r="N55">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -5480,15 +5449,15 @@
       <c r="B56" t="s">
         <v>176</v>
       </c>
-      <c r="C56" s="58"/>
+      <c r="C56" s="52"/>
       <c r="D56" s="1"/>
-      <c r="L56" s="59"/>
+      <c r="L56" s="53"/>
       <c r="N56">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -5496,15 +5465,15 @@
       <c r="B57" t="s">
         <v>176</v>
       </c>
-      <c r="C57" s="58"/>
+      <c r="C57" s="52"/>
       <c r="D57" s="1"/>
-      <c r="L57" s="59"/>
+      <c r="L57" s="53"/>
       <c r="N57">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -5512,15 +5481,15 @@
       <c r="B58" t="s">
         <v>176</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="52"/>
       <c r="D58" s="1"/>
-      <c r="L58" s="59"/>
+      <c r="L58" s="53"/>
       <c r="N58">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -5528,15 +5497,15 @@
       <c r="B59" t="s">
         <v>176</v>
       </c>
-      <c r="C59" s="58"/>
+      <c r="C59" s="52"/>
       <c r="D59" s="1"/>
-      <c r="L59" s="59"/>
+      <c r="L59" s="53"/>
       <c r="N59">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -5544,15 +5513,15 @@
       <c r="B60" t="s">
         <v>176</v>
       </c>
-      <c r="C60" s="58"/>
+      <c r="C60" s="52"/>
       <c r="D60" s="1"/>
-      <c r="L60" s="59"/>
+      <c r="L60" s="53"/>
       <c r="N60">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -5560,15 +5529,15 @@
       <c r="B61" t="s">
         <v>176</v>
       </c>
-      <c r="C61" s="58"/>
+      <c r="C61" s="52"/>
       <c r="D61" s="1"/>
-      <c r="L61" s="59"/>
+      <c r="L61" s="53"/>
       <c r="N61">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -5576,15 +5545,15 @@
       <c r="B62" t="s">
         <v>176</v>
       </c>
-      <c r="C62" s="58"/>
+      <c r="C62" s="52"/>
       <c r="D62" s="1"/>
-      <c r="L62" s="59"/>
+      <c r="L62" s="53"/>
       <c r="N62">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -5592,15 +5561,15 @@
       <c r="B63" t="s">
         <v>176</v>
       </c>
-      <c r="C63" s="58"/>
+      <c r="C63" s="52"/>
       <c r="D63" s="1"/>
-      <c r="L63" s="59"/>
+      <c r="L63" s="53"/>
       <c r="N63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -5608,15 +5577,15 @@
       <c r="B64" t="s">
         <v>176</v>
       </c>
-      <c r="C64" s="58"/>
+      <c r="C64" s="52"/>
       <c r="D64" s="1"/>
-      <c r="L64" s="59"/>
+      <c r="L64" s="53"/>
       <c r="N64">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -5624,15 +5593,15 @@
       <c r="B65" t="s">
         <v>176</v>
       </c>
-      <c r="C65" s="58"/>
+      <c r="C65" s="52"/>
       <c r="D65" s="1"/>
-      <c r="L65" s="59"/>
+      <c r="L65" s="53"/>
       <c r="N65">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -5640,15 +5609,15 @@
       <c r="B66" t="s">
         <v>176</v>
       </c>
-      <c r="C66" s="58"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="1"/>
-      <c r="L66" s="59"/>
+      <c r="L66" s="53"/>
       <c r="N66">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -5656,15 +5625,15 @@
       <c r="B67" t="s">
         <v>176</v>
       </c>
-      <c r="C67" s="58"/>
+      <c r="C67" s="52"/>
       <c r="D67" s="1"/>
-      <c r="L67" s="59"/>
+      <c r="L67" s="53"/>
       <c r="N67">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -5672,15 +5641,15 @@
       <c r="B68" t="s">
         <v>176</v>
       </c>
-      <c r="C68" s="58"/>
+      <c r="C68" s="52"/>
       <c r="D68" s="1"/>
-      <c r="L68" s="59"/>
+      <c r="L68" s="53"/>
       <c r="N68">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -5688,15 +5657,15 @@
       <c r="B69" t="s">
         <v>176</v>
       </c>
-      <c r="C69" s="58"/>
+      <c r="C69" s="52"/>
       <c r="D69" s="1"/>
-      <c r="L69" s="59"/>
+      <c r="L69" s="53"/>
       <c r="N69">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -5704,15 +5673,15 @@
       <c r="B70" t="s">
         <v>176</v>
       </c>
-      <c r="C70" s="58"/>
+      <c r="C70" s="52"/>
       <c r="D70" s="1"/>
-      <c r="L70" s="59"/>
+      <c r="L70" s="53"/>
       <c r="N70">
         <f t="shared" ref="N70:N102" si="12">IF(M70="Y",1500, )</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" ref="A71:A102" si="13">A70+1</f>
         <v>67</v>
@@ -5720,15 +5689,15 @@
       <c r="B71" t="s">
         <v>176</v>
       </c>
-      <c r="C71" s="58"/>
+      <c r="C71" s="52"/>
       <c r="D71" s="1"/>
-      <c r="L71" s="59"/>
+      <c r="L71" s="53"/>
       <c r="N71">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="13"/>
         <v>68</v>
@@ -5736,15 +5705,15 @@
       <c r="B72" t="s">
         <v>176</v>
       </c>
-      <c r="C72" s="58"/>
+      <c r="C72" s="52"/>
       <c r="D72" s="1"/>
-      <c r="L72" s="59"/>
+      <c r="L72" s="53"/>
       <c r="N72">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="13"/>
         <v>69</v>
@@ -5752,15 +5721,15 @@
       <c r="B73" t="s">
         <v>176</v>
       </c>
-      <c r="C73" s="58"/>
+      <c r="C73" s="52"/>
       <c r="D73" s="1"/>
-      <c r="L73" s="59"/>
+      <c r="L73" s="53"/>
       <c r="N73">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="13"/>
         <v>70</v>
@@ -5768,15 +5737,15 @@
       <c r="B74" t="s">
         <v>176</v>
       </c>
-      <c r="C74" s="58"/>
+      <c r="C74" s="52"/>
       <c r="D74" s="1"/>
-      <c r="L74" s="59"/>
+      <c r="L74" s="53"/>
       <c r="N74">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="13"/>
         <v>71</v>
@@ -5784,15 +5753,15 @@
       <c r="B75" t="s">
         <v>176</v>
       </c>
-      <c r="C75" s="58"/>
+      <c r="C75" s="52"/>
       <c r="D75" s="1"/>
-      <c r="L75" s="59"/>
+      <c r="L75" s="53"/>
       <c r="N75">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="13"/>
         <v>72</v>
@@ -5800,15 +5769,15 @@
       <c r="B76" t="s">
         <v>176</v>
       </c>
-      <c r="C76" s="58"/>
+      <c r="C76" s="52"/>
       <c r="D76" s="1"/>
-      <c r="L76" s="59"/>
+      <c r="L76" s="53"/>
       <c r="N76">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="13"/>
         <v>73</v>
@@ -5816,12 +5785,12 @@
       <c r="B77" t="s">
         <v>176</v>
       </c>
-      <c r="C77" s="58"/>
+      <c r="C77" s="52"/>
       <c r="D77" s="1"/>
       <c r="K77" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L77" s="59"/>
+      <c r="L77" s="53"/>
       <c r="M77" s="1" t="s">
         <v>177</v>
       </c>
@@ -5830,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="13"/>
         <v>74</v>
@@ -5838,15 +5807,15 @@
       <c r="B78" t="s">
         <v>176</v>
       </c>
-      <c r="C78" s="58"/>
+      <c r="C78" s="52"/>
       <c r="D78" s="1"/>
-      <c r="L78" s="59"/>
+      <c r="L78" s="53"/>
       <c r="N78">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="13"/>
         <v>75</v>
@@ -5854,15 +5823,15 @@
       <c r="B79" t="s">
         <v>176</v>
       </c>
-      <c r="C79" s="58"/>
+      <c r="C79" s="52"/>
       <c r="D79" s="1"/>
-      <c r="L79" s="59"/>
+      <c r="L79" s="53"/>
       <c r="N79">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="13"/>
         <v>76</v>
@@ -5870,15 +5839,15 @@
       <c r="B80" t="s">
         <v>176</v>
       </c>
-      <c r="C80" s="58"/>
+      <c r="C80" s="52"/>
       <c r="D80" s="1"/>
-      <c r="L80" s="59"/>
+      <c r="L80" s="53"/>
       <c r="N80">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="13"/>
         <v>77</v>
@@ -5886,14 +5855,14 @@
       <c r="B81" t="s">
         <v>176</v>
       </c>
-      <c r="C81" s="58"/>
+      <c r="C81" s="52"/>
       <c r="D81" s="1"/>
       <c r="N81">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="13"/>
         <v>78</v>
@@ -5901,14 +5870,14 @@
       <c r="B82" t="s">
         <v>176</v>
       </c>
-      <c r="C82" s="58"/>
+      <c r="C82" s="52"/>
       <c r="D82" s="1"/>
       <c r="N82">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="13"/>
         <v>79</v>
@@ -5916,14 +5885,14 @@
       <c r="B83" t="s">
         <v>176</v>
       </c>
-      <c r="C83" s="58"/>
+      <c r="C83" s="52"/>
       <c r="D83" s="1"/>
       <c r="N83">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="13"/>
         <v>80</v>
@@ -5931,14 +5900,14 @@
       <c r="B84" t="s">
         <v>176</v>
       </c>
-      <c r="C84" s="58"/>
+      <c r="C84" s="52"/>
       <c r="D84" s="1"/>
       <c r="N84">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="13"/>
         <v>81</v>
@@ -5946,14 +5915,14 @@
       <c r="B85" t="s">
         <v>176</v>
       </c>
-      <c r="C85" s="58"/>
+      <c r="C85" s="52"/>
       <c r="D85" s="1"/>
       <c r="N85">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="13"/>
         <v>82</v>
@@ -5961,14 +5930,14 @@
       <c r="B86" t="s">
         <v>176</v>
       </c>
-      <c r="C86" s="58"/>
+      <c r="C86" s="52"/>
       <c r="D86" s="1"/>
       <c r="N86">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="13"/>
         <v>83</v>
@@ -5976,14 +5945,14 @@
       <c r="B87" t="s">
         <v>176</v>
       </c>
-      <c r="C87" s="58"/>
+      <c r="C87" s="52"/>
       <c r="D87" s="1"/>
       <c r="N87">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="13"/>
         <v>84</v>
@@ -5991,14 +5960,14 @@
       <c r="B88" t="s">
         <v>176</v>
       </c>
-      <c r="C88" s="58"/>
+      <c r="C88" s="52"/>
       <c r="D88" s="1"/>
       <c r="N88">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="13"/>
         <v>85</v>
@@ -6006,14 +5975,14 @@
       <c r="B89" t="s">
         <v>176</v>
       </c>
-      <c r="C89" s="58"/>
+      <c r="C89" s="52"/>
       <c r="D89" s="1"/>
       <c r="N89">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="13"/>
         <v>86</v>
@@ -6021,14 +5990,14 @@
       <c r="B90" t="s">
         <v>176</v>
       </c>
-      <c r="C90" s="58"/>
+      <c r="C90" s="52"/>
       <c r="D90" s="1"/>
       <c r="N90">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="13"/>
         <v>87</v>
@@ -6036,14 +6005,14 @@
       <c r="B91" t="s">
         <v>176</v>
       </c>
-      <c r="C91" s="58"/>
+      <c r="C91" s="52"/>
       <c r="D91" s="1"/>
       <c r="N91">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="13"/>
         <v>88</v>
@@ -6051,14 +6020,14 @@
       <c r="B92" t="s">
         <v>176</v>
       </c>
-      <c r="C92" s="58"/>
+      <c r="C92" s="52"/>
       <c r="D92" s="1"/>
       <c r="N92">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="13"/>
         <v>89</v>
@@ -6066,14 +6035,14 @@
       <c r="B93" t="s">
         <v>176</v>
       </c>
-      <c r="C93" s="58"/>
+      <c r="C93" s="52"/>
       <c r="D93" s="1"/>
       <c r="N93">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="13"/>
         <v>90</v>
@@ -6081,14 +6050,14 @@
       <c r="B94" t="s">
         <v>176</v>
       </c>
-      <c r="C94" s="58"/>
+      <c r="C94" s="52"/>
       <c r="D94" s="1"/>
       <c r="N94">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="13"/>
         <v>91</v>
@@ -6096,14 +6065,14 @@
       <c r="B95" t="s">
         <v>176</v>
       </c>
-      <c r="C95" s="58"/>
+      <c r="C95" s="52"/>
       <c r="D95" s="1"/>
       <c r="N95">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <f t="shared" si="13"/>
         <v>92</v>
@@ -6111,14 +6080,14 @@
       <c r="B96" t="s">
         <v>176</v>
       </c>
-      <c r="C96" s="58"/>
+      <c r="C96" s="52"/>
       <c r="D96" s="1"/>
       <c r="N96">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <f t="shared" si="13"/>
         <v>93</v>
@@ -6126,14 +6095,14 @@
       <c r="B97" t="s">
         <v>176</v>
       </c>
-      <c r="C97" s="58"/>
+      <c r="C97" s="52"/>
       <c r="D97" s="1"/>
       <c r="N97">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <f t="shared" si="13"/>
         <v>94</v>
@@ -6141,14 +6110,14 @@
       <c r="B98" t="s">
         <v>176</v>
       </c>
-      <c r="C98" s="58"/>
+      <c r="C98" s="52"/>
       <c r="D98" s="1"/>
       <c r="N98">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <f t="shared" si="13"/>
         <v>95</v>
@@ -6156,14 +6125,14 @@
       <c r="B99" t="s">
         <v>176</v>
       </c>
-      <c r="C99" s="58"/>
+      <c r="C99" s="52"/>
       <c r="D99" s="1"/>
       <c r="N99">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <f t="shared" si="13"/>
         <v>96</v>
@@ -6171,14 +6140,14 @@
       <c r="B100" t="s">
         <v>176</v>
       </c>
-      <c r="C100" s="58"/>
+      <c r="C100" s="52"/>
       <c r="D100" s="1"/>
       <c r="N100">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <f t="shared" si="13"/>
         <v>97</v>
@@ -6186,14 +6155,14 @@
       <c r="B101" t="s">
         <v>176</v>
       </c>
-      <c r="C101" s="58"/>
+      <c r="C101" s="52"/>
       <c r="D101" s="1"/>
       <c r="N101">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <f t="shared" si="13"/>
         <v>98</v>
@@ -6201,14 +6170,14 @@
       <c r="B102" t="s">
         <v>176</v>
       </c>
-      <c r="C102" s="58"/>
+      <c r="C102" s="52"/>
       <c r="D102" s="1"/>
       <c r="N102">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="141" t="s">
         <v>178</v>
       </c>
@@ -6232,33 +6201,33 @@
       <c r="S104" s="142"/>
       <c r="T104" s="142"/>
     </row>
-    <row r="105" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="60"/>
-      <c r="B105" s="61"/>
-      <c r="C105" s="61"/>
-      <c r="D105" s="61"/>
-      <c r="E105" s="61"/>
-      <c r="F105" s="61"/>
-      <c r="G105" s="61"/>
-      <c r="H105" s="61"/>
-      <c r="I105" s="61"/>
-      <c r="J105" s="61"/>
-      <c r="K105" s="61"/>
-      <c r="L105" s="61"/>
-      <c r="M105" s="61"/>
-      <c r="N105" s="61"/>
-      <c r="O105" s="61"/>
-      <c r="P105" s="61"/>
-      <c r="Q105" s="61"/>
-      <c r="R105" s="61"/>
-      <c r="S105" s="61"/>
-      <c r="T105" s="61"/>
-    </row>
-    <row r="106" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="54"/>
+      <c r="B105" s="55"/>
+      <c r="C105" s="55"/>
+      <c r="D105" s="55"/>
+      <c r="E105" s="55"/>
+      <c r="F105" s="55"/>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="55"/>
+      <c r="J105" s="55"/>
+      <c r="K105" s="55"/>
+      <c r="L105" s="55"/>
+      <c r="M105" s="55"/>
+      <c r="N105" s="55"/>
+      <c r="O105" s="55"/>
+      <c r="P105" s="55"/>
+      <c r="Q105" s="55"/>
+      <c r="R105" s="55"/>
+      <c r="S105" s="55"/>
+      <c r="T105" s="55"/>
+    </row>
+    <row r="106" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>30</v>
       </c>
-      <c r="C106" s="62" t="s">
+      <c r="C106" s="56" t="s">
         <v>179</v>
       </c>
       <c r="D106">
@@ -6273,13 +6242,13 @@
       <c r="G106" t="s">
         <v>180</v>
       </c>
-      <c r="P106" s="63">
+      <c r="P106" s="57">
         <v>22019</v>
       </c>
       <c r="S106">
         <v>6266167273</v>
       </c>
-      <c r="T106" s="64" t="s">
+      <c r="T106" s="58" t="s">
         <v>181</v>
       </c>
       <c r="U106">
@@ -6289,11 +6258,11 @@
         <v>128934</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>30</v>
       </c>
-      <c r="C107" s="62" t="s">
+      <c r="C107" s="56" t="s">
         <v>182</v>
       </c>
       <c r="D107">
@@ -6308,13 +6277,13 @@
       <c r="G107" t="s">
         <v>180</v>
       </c>
-      <c r="P107" s="63">
+      <c r="P107" s="57">
         <v>21789</v>
       </c>
       <c r="S107" t="s">
         <v>184</v>
       </c>
-      <c r="T107" s="64" t="s">
+      <c r="T107" s="58" t="s">
         <v>185</v>
       </c>
       <c r="U107">
@@ -6324,32 +6293,29 @@
         <v>273727</v>
       </c>
     </row>
-    <row r="108" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C108" s="62"/>
-    </row>
-    <row r="109" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C109" s="62"/>
-    </row>
-    <row r="110" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C110" s="62"/>
-    </row>
-    <row r="111" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C111" s="62"/>
-    </row>
-    <row r="112" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C112" s="62"/>
-    </row>
-    <row r="113" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C113" s="62"/>
-    </row>
-    <row r="114" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C114" s="62"/>
-    </row>
-    <row r="115" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C115" s="62"/>
+    <row r="108" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="C108" s="56"/>
+    </row>
+    <row r="109" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="C109" s="56"/>
+    </row>
+    <row r="110" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="C110" s="56"/>
+    </row>
+    <row r="111" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="C111" s="56"/>
+    </row>
+    <row r="112" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="C112" s="56"/>
+    </row>
+    <row r="113" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C113" s="56"/>
+    </row>
+    <row r="114" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C114" s="56"/>
+    </row>
+    <row r="115" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="C115" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6537,33 +6503,33 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" customWidth="1"/>
-    <col min="3" max="3" width="0.7265625" customWidth="1"/>
-    <col min="4" max="4" width="3.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="0.7109375" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="0.7265625" customWidth="1"/>
-    <col min="9" max="9" width="5.26953125" customWidth="1"/>
-    <col min="10" max="10" width="5.81640625" customWidth="1"/>
-    <col min="11" max="11" width="5.1796875" customWidth="1"/>
+    <col min="8" max="8" width="0.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
     <col min="13" max="13" width="1" customWidth="1"/>
-    <col min="14" max="14" width="7.54296875" customWidth="1"/>
-    <col min="15" max="15" width="10.7265625" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" customWidth="1"/>
-    <col min="17" max="17" width="5.81640625" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" customWidth="1"/>
-    <col min="19" max="19" width="29.54296875" customWidth="1"/>
-    <col min="20" max="20" width="34.7265625" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" customWidth="1"/>
+    <col min="19" max="19" width="29.5703125" customWidth="1"/>
+    <col min="20" max="20" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="144"/>
       <c r="C1" s="144"/>
@@ -6583,10 +6549,10 @@
       <c r="Q1" s="144"/>
       <c r="R1" s="144"/>
       <c r="S1" s="144"/>
-      <c r="T1" s="65"/>
-    </row>
-    <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="66"/>
+      <c r="T1" s="59"/>
+    </row>
+    <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
       <c r="B2" s="137" t="s">
         <v>1</v>
       </c>
@@ -6594,13 +6560,13 @@
       <c r="D2" s="137"/>
       <c r="E2" s="138">
         <f ca="1">(TODAY())</f>
-        <v>46059</v>
+        <v>46061</v>
       </c>
       <c r="F2" s="138"/>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="68">
+      <c r="I2" s="62">
         <f>COUNTA(B4:B17)</f>
         <v>5</v>
       </c>
@@ -6613,111 +6579,111 @@
       </c>
       <c r="L2" s="145"/>
       <c r="M2" s="145"/>
-      <c r="N2" s="69">
+      <c r="N2" s="63">
         <f>COUNTIF(D4:D14, "M")</f>
         <v>5</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="70">
+      <c r="P2" s="64">
         <f>COUNTIF(D4:D17, "F")</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="71" t="s">
-        <v>188</v>
-      </c>
-      <c r="R2" s="72">
+      <c r="Q2" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="R2" s="66">
         <f>COUNTIF(L4:L17, "H")</f>
         <v>3</v>
       </c>
-      <c r="T2" s="65"/>
-    </row>
-    <row r="3" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73" t="s">
+      <c r="T2" s="59"/>
+    </row>
+    <row r="3" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="76" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="77" t="s">
+      <c r="I3" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="68" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="76" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="74" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="74" t="s">
+      <c r="L3" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="L3" s="76" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="76" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="T3" s="65"/>
-    </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="79"/>
-      <c r="C4" s="58"/>
+      <c r="T3" s="59"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="73"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="1"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="80"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="6"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="80"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="74"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="T4" s="65"/>
-    </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="79">
+      <c r="T4" s="59"/>
+    </row>
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="73">
         <f>A4+1</f>
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="1" t="s">
         <v>36</v>
       </c>
@@ -6727,47 +6693,47 @@
       <c r="F5" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="57">
         <v>45890</v>
       </c>
-      <c r="H5" s="80"/>
+      <c r="H5" s="74"/>
       <c r="I5" s="6">
         <f t="shared" ref="I5:I6" ca="1" si="0">IF(G5="","",IF(H5="",TODAY()-G5,DATEDIF(G5,H5,"d")))</f>
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="59"/>
-      <c r="L5" s="81" t="s">
-        <v>193</v>
-      </c>
-      <c r="M5" s="80"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="75" t="s">
+        <v>192</v>
+      </c>
+      <c r="M5" s="74"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="63">
+      <c r="O5" s="57">
         <v>31961</v>
       </c>
-      <c r="P5" s="63">
+      <c r="P5" s="57">
         <v>45887</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" ref="Q5:Q6" ca="1" si="1">IF(P5="","",(TODAY()-P5))</f>
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="T5" s="65"/>
-    </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="79">
+      <c r="T5" s="59"/>
+    </row>
+    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="73">
         <f t="shared" ref="A6" si="2">A5+1</f>
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
@@ -6775,118 +6741,118 @@
         <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G6" s="63">
+        <v>193</v>
+      </c>
+      <c r="G6" s="57">
         <v>45891</v>
       </c>
-      <c r="H6" s="80"/>
+      <c r="H6" s="74"/>
       <c r="I6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="81" t="s">
-        <v>193</v>
-      </c>
-      <c r="M6" s="80"/>
+      <c r="L6" s="75" t="s">
+        <v>192</v>
+      </c>
+      <c r="M6" s="74"/>
       <c r="N6" s="1"/>
-      <c r="P6" s="63">
+      <c r="P6" s="57">
         <v>45750</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="R6" s="1"/>
-      <c r="T6" s="65"/>
-    </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="79">
+      <c r="T6" s="59"/>
+    </row>
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="73">
         <v>3</v>
       </c>
-      <c r="B7" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="83" t="s">
+      <c r="B7" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="76"/>
+      <c r="D7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="F7" s="82" t="s">
+      <c r="F7" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="G7" s="63">
+      <c r="G7" s="57">
         <v>45936</v>
       </c>
       <c r="I7" s="1">
         <f ca="1">IF(G7="","",IF(H7="",TODAY()-G7,DATEDIF(G7,H7,"d")))</f>
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="59" t="s">
-        <v>196</v>
+      <c r="K7" s="53" t="s">
+        <v>195</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>138</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="63">
+      <c r="O7" s="57">
         <v>34191</v>
       </c>
-      <c r="P7" s="63">
+      <c r="P7" s="57">
         <v>45941</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" ref="Q7:Q8" ca="1" si="3">IF(P7="","",(TODAY()-P7))</f>
-        <v>118</v>
-      </c>
-      <c r="R7" s="82" t="s">
+        <v>120</v>
+      </c>
+      <c r="R7" s="76" t="s">
         <v>169</v>
       </c>
-      <c r="S7" s="64" t="s">
+      <c r="S7" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="T7" s="65"/>
-    </row>
-    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="79">
+      <c r="T7" s="59"/>
+    </row>
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="73">
         <f t="shared" ref="A8:A13" si="4">A7+1</f>
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D8" s="82" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="82" t="s">
+      <c r="E8" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="G8" s="63">
+      <c r="G8" s="57">
         <v>45954</v>
       </c>
       <c r="I8" s="6">
         <f ca="1">IF(G8="","",IF(H8="",TODAY()-G8,DATEDIF(G8,H8,"d")))</f>
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="59" t="s">
-        <v>198</v>
+      <c r="K8" s="53" t="s">
+        <v>197</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>138</v>
@@ -6895,30 +6861,30 @@
         <v>1500</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="63">
+      <c r="O8" s="57">
         <v>30045</v>
       </c>
-      <c r="P8" s="63">
+      <c r="P8" s="57">
         <v>45860</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>199</v>
-      </c>
-      <c r="S8" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="S8" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="T8" s="65"/>
-    </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="79">
+      <c r="T8" s="59"/>
+    </row>
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="73">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C9" s="58">
+        <v>198</v>
+      </c>
+      <c r="C9" s="52">
         <v>135</v>
       </c>
       <c r="D9" t="s">
@@ -6930,18 +6896,18 @@
       <c r="F9" t="s">
         <v>160</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="57">
         <v>45982</v>
       </c>
-      <c r="H9" s="63"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="1">
         <f t="shared" ref="I9" ca="1" si="5">IF(G9="","",IF(H9="",TODAY()-G9,DATEDIF(G9,H9,"d")))</f>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="K9" s="53" t="s">
         <v>161</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -6951,124 +6917,124 @@
         <v>1500</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="63">
+      <c r="O9" s="57">
         <v>32216</v>
       </c>
-      <c r="P9" s="63">
+      <c r="P9" s="57">
         <v>45853</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" ref="Q9" ca="1" si="6">IF(P9="","",(TODAY()-P9))</f>
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="R9" t="s">
         <v>162</v>
       </c>
-      <c r="T9" s="65"/>
-    </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="79">
+      <c r="T9" s="59"/>
+    </row>
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="73">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="T10" s="65"/>
-    </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="79">
+      <c r="T10" s="59"/>
+    </row>
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="73">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="T11" s="65"/>
-    </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="79">
+      <c r="T11" s="59"/>
+    </row>
+    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="73">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="T12" s="65"/>
-    </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="79">
+      <c r="T12" s="59"/>
+    </row>
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="73">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="G13" s="63"/>
+      <c r="G13" s="57"/>
       <c r="I13" s="6"/>
       <c r="J13" s="1"/>
-      <c r="L13" s="81"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
+      <c r="L13" s="75"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="65"/>
-    </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="84">
+      <c r="S13" s="58"/>
+      <c r="T13" s="59"/>
+    </row>
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="78">
         <v>14</v>
       </c>
-      <c r="T14" s="65"/>
-    </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="85"/>
-      <c r="B15" s="85"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="86" t="s">
+      <c r="T14" s="59"/>
+    </row>
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="87" t="s">
+      <c r="F15" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="85"/>
-      <c r="P15" s="85"/>
-      <c r="Q15" s="85"/>
-      <c r="R15" s="85"/>
-      <c r="S15" s="85"/>
-      <c r="T15" s="65"/>
-    </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K16" s="62"/>
-      <c r="L16" s="91"/>
-      <c r="M16" s="80"/>
-    </row>
-    <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K17" s="62"/>
-      <c r="L17" s="82"/>
-    </row>
-    <row r="18" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="63"/>
-      <c r="K18" s="62"/>
-    </row>
-    <row r="19" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="K19" s="62"/>
-    </row>
-    <row r="20" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="79"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="59"/>
+    </row>
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="56"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="74"/>
+    </row>
+    <row r="17" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="K17" s="56"/>
+      <c r="L17" s="76"/>
+    </row>
+    <row r="18" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="57"/>
+      <c r="K18" s="56"/>
+    </row>
+    <row r="19" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="K19" s="56"/>
+    </row>
+    <row r="20" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E20" t="str">
         <f t="array" aca="1" ref="E20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
         <v>James</v>
       </c>
-      <c r="F20" t="str">
+      <c r="F20">
         <f t="array" aca="1" ref="F20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
-        <v>James</v>
-      </c>
-      <c r="K20" s="62"/>
-    </row>
-    <row r="21" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K21" s="62"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="56"/>
+    </row>
+    <row r="21" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="K21" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7124,22 +7090,22 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" customWidth="1"/>
-    <col min="2" max="2" width="6.54296875" customWidth="1"/>
-    <col min="3" max="3" width="2.54296875" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="3.453125" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="9" max="9" width="1.453125" customWidth="1"/>
+    <col min="9" max="9" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="92"/>
+    <row r="1" spans="1:9" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="86"/>
       <c r="B1" s="170" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C1" s="171"/>
       <c r="D1" s="171"/>
@@ -7147,295 +7113,295 @@
       <c r="F1" s="171"/>
       <c r="G1" s="171"/>
       <c r="H1" s="171"/>
-      <c r="I1" s="92"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="92"/>
+      <c r="I1" s="86"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="86"/>
       <c r="B2" s="172" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="173"/>
       <c r="D2" s="174"/>
-      <c r="E2" s="93"/>
+      <c r="E2" s="87"/>
       <c r="F2" s="175" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G2" s="176"/>
       <c r="H2" s="177"/>
       <c r="I2" s="178"/>
     </row>
-    <row r="3" spans="1:9" ht="5.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="92"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99"/>
+    <row r="3" spans="1:9" ht="5.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="86"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="178"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="92"/>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="86"/>
       <c r="B4" s="152" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="D4" s="96"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="165" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="165" t="s">
+      <c r="G4" s="97" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="86"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="86"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="99" t="s">
         <v>206</v>
       </c>
-      <c r="G4" s="103" t="s">
-        <v>205</v>
-      </c>
-      <c r="H4" s="104" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="92"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="92"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="105" t="s">
+      <c r="D5" s="100"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="166"/>
+      <c r="G5" s="101" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="86"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="86"/>
+      <c r="B6" s="154"/>
+      <c r="C6" s="103" t="s">
         <v>207</v>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="166"/>
-      <c r="G5" s="107" t="s">
+      <c r="D6" s="104"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="167"/>
+      <c r="G6" s="103" t="s">
         <v>207</v>
       </c>
-      <c r="H5" s="108" t="s">
-        <v>172</v>
-      </c>
-      <c r="I5" s="92"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="92"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="109" t="s">
+      <c r="H6" s="105"/>
+      <c r="I6" s="86"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="86"/>
+      <c r="B7" s="152" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="167"/>
-      <c r="G6" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="H6" s="111"/>
-      <c r="I6" s="92"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="92"/>
-      <c r="B7" s="152" t="s">
+      <c r="C7" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="106"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="165" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="101" t="s">
-        <v>205</v>
-      </c>
-      <c r="D7" s="112"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="165" t="s">
+      <c r="G7" s="97" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="98"/>
+      <c r="I7" s="86"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="86"/>
+      <c r="B8" s="153"/>
+      <c r="C8" s="99" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="107"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="101" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="86"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="86"/>
+      <c r="B9" s="154"/>
+      <c r="C9" s="103" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="105"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="103" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" s="105"/>
+      <c r="I9" s="86"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="86"/>
+      <c r="B10" s="152" t="s">
         <v>210</v>
       </c>
-      <c r="G7" s="103" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="104"/>
-      <c r="I7" s="92"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="92"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="105" t="s">
+      <c r="C10" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="106"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="168" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="108" t="s">
+        <v>204</v>
+      </c>
+      <c r="H10" s="109"/>
+      <c r="I10" s="86"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="86"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="99" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="107"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="169"/>
+      <c r="G11" s="110" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="111"/>
+      <c r="I11" s="86"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="86"/>
+      <c r="B12" s="154"/>
+      <c r="C12" s="112" t="s">
         <v>207</v>
       </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="107" t="s">
+      <c r="D12" s="113"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="168" t="s">
+        <v>212</v>
+      </c>
+      <c r="G12" s="97" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12" s="92" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" s="86"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="86"/>
+      <c r="B13" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="106"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="101" t="s">
+        <v>206</v>
+      </c>
+      <c r="H13" s="102" t="s">
+        <v>214</v>
+      </c>
+      <c r="I13" s="86"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="86"/>
+      <c r="B14" s="152" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" s="115"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="103" t="s">
         <v>207</v>
       </c>
-      <c r="H8" s="108" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="92"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="92"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="D9" s="111"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="167"/>
-      <c r="G9" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="111"/>
-      <c r="I9" s="92"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="92"/>
-      <c r="B10" s="152" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" s="101" t="s">
-        <v>205</v>
-      </c>
-      <c r="D10" s="112"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="168" t="s">
-        <v>212</v>
-      </c>
-      <c r="G10" s="114" t="s">
-        <v>205</v>
-      </c>
-      <c r="H10" s="115"/>
-      <c r="I10" s="92"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="92"/>
-      <c r="B11" s="153"/>
-      <c r="C11" s="105" t="s">
+      <c r="H14" s="105"/>
+      <c r="I14" s="86"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="86"/>
+      <c r="B15" s="153"/>
+      <c r="C15" s="117" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="118"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="155"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="86"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="86"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="103" t="s">
         <v>207</v>
       </c>
-      <c r="D11" s="113"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="169"/>
-      <c r="G11" s="116" t="s">
-        <v>207</v>
-      </c>
-      <c r="H11" s="117"/>
-      <c r="I11" s="92"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="92"/>
-      <c r="B12" s="154"/>
-      <c r="C12" s="118" t="s">
-        <v>208</v>
-      </c>
-      <c r="D12" s="119"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="168" t="s">
-        <v>213</v>
-      </c>
-      <c r="G12" s="103" t="s">
-        <v>205</v>
-      </c>
-      <c r="H12" s="98" t="s">
-        <v>159</v>
-      </c>
-      <c r="I12" s="92"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="92"/>
-      <c r="B13" s="100" t="s">
-        <v>214</v>
-      </c>
-      <c r="C13" s="101" t="s">
-        <v>205</v>
-      </c>
-      <c r="D13" s="112"/>
-      <c r="E13" s="92"/>
-      <c r="F13" s="169"/>
-      <c r="G13" s="107" t="s">
-        <v>207</v>
-      </c>
-      <c r="H13" s="108" t="s">
-        <v>215</v>
-      </c>
-      <c r="I13" s="92"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="92"/>
-      <c r="B14" s="152" t="s">
+      <c r="D16" s="105"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="86"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="86"/>
+      <c r="B17" s="158" t="s">
         <v>216</v>
       </c>
-      <c r="C14" s="120" t="s">
-        <v>205</v>
-      </c>
-      <c r="D14" s="121"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="122"/>
-      <c r="G14" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="H14" s="111"/>
-      <c r="I14" s="92"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="92"/>
-      <c r="B15" s="153"/>
-      <c r="C15" s="123" t="s">
-        <v>207</v>
-      </c>
-      <c r="D15" s="124"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="155"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="121"/>
-      <c r="I15" s="92"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="92"/>
-      <c r="B16" s="154"/>
-      <c r="C16" s="109" t="s">
-        <v>208</v>
-      </c>
-      <c r="D16" s="111"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="92"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="92"/>
-      <c r="B17" s="158" t="s">
+      <c r="C17" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="115"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="86"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="86"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="117" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" s="118"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="121"/>
+      <c r="I18" s="86"/>
+    </row>
+    <row r="19" spans="1:9" ht="9.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="86"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+    </row>
+    <row r="20" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="160" t="s">
         <v>217</v>
-      </c>
-      <c r="C17" s="120" t="s">
-        <v>205</v>
-      </c>
-      <c r="D17" s="121"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="157"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="92"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="92"/>
-      <c r="B18" s="159"/>
-      <c r="C18" s="123" t="s">
-        <v>207</v>
-      </c>
-      <c r="D18" s="124"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="92"/>
-    </row>
-    <row r="19" spans="1:9" ht="9.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="92"/>
-      <c r="B19" s="92"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="92"/>
-    </row>
-    <row r="20" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="160" t="s">
-        <v>218</v>
       </c>
       <c r="B20" s="160"/>
       <c r="C20" s="160"/>
@@ -7446,7 +7412,7 @@
       <c r="H20" s="160"/>
       <c r="I20" s="160"/>
     </row>
-    <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="160"/>
       <c r="B21" s="160"/>
       <c r="C21" s="160"/>
@@ -7457,79 +7423,79 @@
       <c r="H21" s="160"/>
       <c r="I21" s="160"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="92"/>
-      <c r="B22" s="128" t="s">
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="86"/>
+      <c r="B22" s="122" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" s="161" t="s">
         <v>219</v>
       </c>
-      <c r="C22" s="161" t="s">
-        <v>220</v>
-      </c>
       <c r="D22" s="162"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="130" t="s">
+      <c r="E22" s="123"/>
+      <c r="F22" s="124" t="s">
+        <v>218</v>
+      </c>
+      <c r="G22" s="163" t="s">
         <v>219</v>
       </c>
-      <c r="G22" s="163" t="s">
-        <v>220</v>
-      </c>
       <c r="H22" s="164"/>
-      <c r="I22" s="92"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="92"/>
-      <c r="B23" s="131"/>
+      <c r="I22" s="86"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="86"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="149"/>
       <c r="D23" s="149"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="132"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="126"/>
       <c r="G23" s="150"/>
       <c r="H23" s="151"/>
-      <c r="I23" s="92"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="92"/>
-      <c r="B24" s="133"/>
+      <c r="I23" s="86"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="86"/>
+      <c r="B24" s="127"/>
       <c r="C24" s="146"/>
       <c r="D24" s="146"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="134"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="128"/>
       <c r="G24" s="147"/>
       <c r="H24" s="148"/>
-      <c r="I24" s="92"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="92"/>
-      <c r="B25" s="133"/>
+      <c r="I24" s="86"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="86"/>
+      <c r="B25" s="127"/>
       <c r="C25" s="146"/>
       <c r="D25" s="146"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="134"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="128"/>
       <c r="G25" s="147"/>
       <c r="H25" s="148"/>
-      <c r="I25" s="92"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="92"/>
-      <c r="B26" s="133"/>
+      <c r="I25" s="86"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="86"/>
+      <c r="B26" s="127"/>
       <c r="C26" s="146"/>
       <c r="D26" s="146"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="134"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="128"/>
       <c r="G26" s="147"/>
       <c r="H26" s="148"/>
-      <c r="I26" s="92"/>
-    </row>
-    <row r="27" spans="1:9" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="92"/>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="92"/>
+      <c r="I26" s="86"/>
+    </row>
+    <row r="27" spans="1:9" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="86"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>

<commit_message>
Add 'What Makes Us Different' page, update home and why-sober-living-matters with button, improve email campaign
</commit_message>
<xml_diff>
--- a/members .xlsx
+++ b/members .xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29725"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{B7497AC0-A7B1-4A41-910A-4EC7CFA4F027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7B1937D-6B92-4F47-A78F-85135F12C706}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{B7497AC0-A7B1-4A41-910A-4EC7CFA4F027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F83A87B5-DE5D-4532-8D43-C6C7C932678B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="223">
   <si>
     <t>HORIZON-HOUSE MASTER LIST</t>
   </si>
@@ -616,9 +616,6 @@
     <t>hallowell.kirk@gmail.com</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>26-</t>
   </si>
   <si>
@@ -752,6 +749,15 @@
   </si>
   <si>
     <t>0802</t>
+  </si>
+  <si>
+    <t>Tokeski</t>
+  </si>
+  <si>
+    <t>909-548-5138</t>
+  </si>
+  <si>
+    <t>ryantokeski5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1453,10 +1459,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1761,6 +1768,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1791,6 +1799,87 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1809,89 +1898,9 @@
     <xf numFmtId="0" fontId="19" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="44">
@@ -2380,6 +2389,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2699,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2728,40 +2741,40 @@
   <sheetData>
     <row r="1" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="136" t="s">
+      <c r="B1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
-      <c r="Q1" s="136"/>
-      <c r="R1" s="136"/>
-      <c r="S1" s="136"/>
-      <c r="T1" s="136"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="137"/>
+      <c r="P1" s="137"/>
+      <c r="Q1" s="137"/>
+      <c r="R1" s="137"/>
+      <c r="S1" s="137"/>
+      <c r="T1" s="137"/>
     </row>
     <row r="2" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="138">
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="139">
         <f ca="1">(TODAY())</f>
-        <v>46061</v>
-      </c>
-      <c r="G2" s="138"/>
+        <v>46062</v>
+      </c>
+      <c r="G2" s="139"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
@@ -2795,14 +2808,14 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
@@ -2911,7 +2924,7 @@
       </c>
       <c r="J5" s="25">
         <f ca="1">(TODAY()-H5)</f>
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>33</v>
@@ -2990,7 +3003,7 @@
       </c>
       <c r="R6" s="31">
         <f ca="1">IF(Q6="","",(TODAY()-Q6))</f>
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
@@ -3152,7 +3165,7 @@
       </c>
       <c r="R9" s="31">
         <f ca="1">IF(Q9="","",(TODAY()-Q9))</f>
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="S9" s="23"/>
       <c r="T9" s="23" t="s">
@@ -3214,7 +3227,7 @@
       </c>
       <c r="R10" s="31">
         <f t="shared" ref="R10:R33" ca="1" si="4">IF(Q10="","",(TODAY()-Q10))</f>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
@@ -3383,7 +3396,7 @@
       </c>
       <c r="R13" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
@@ -3441,7 +3454,7 @@
       </c>
       <c r="R14" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
@@ -3499,7 +3512,7 @@
       </c>
       <c r="R15" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S15" s="23" t="s">
         <v>65</v>
@@ -3559,7 +3572,7 @@
       </c>
       <c r="R16" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="S16" s="23" t="s">
         <v>70</v>
@@ -3723,7 +3736,7 @@
       </c>
       <c r="R19" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="S19" s="23" t="s">
         <v>79</v>
@@ -3760,7 +3773,7 @@
       <c r="I20" s="39"/>
       <c r="J20" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K20" s="41" t="s">
         <v>50</v>
@@ -3781,12 +3794,15 @@
       </c>
       <c r="R20" s="41">
         <f t="shared" ca="1" si="4"/>
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="S20" s="39" t="s">
         <v>84</v>
       </c>
       <c r="T20" s="39"/>
+      <c r="U20">
+        <v>1556</v>
+      </c>
     </row>
     <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -3839,7 +3855,7 @@
       </c>
       <c r="R21" s="25">
         <f t="shared" ca="1" si="4"/>
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
@@ -3896,7 +3912,7 @@
       </c>
       <c r="R22" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
@@ -3955,7 +3971,7 @@
       </c>
       <c r="R23" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="S23" s="23"/>
       <c r="T23" s="46" t="s">
@@ -4012,7 +4028,7 @@
       </c>
       <c r="R24" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="S24" s="23" t="s">
         <v>99</v>
@@ -4071,7 +4087,7 @@
       </c>
       <c r="R25" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="S25" s="23" t="s">
         <v>103</v>
@@ -4130,7 +4146,7 @@
       </c>
       <c r="R26" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="S26" s="23"/>
       <c r="T26" s="46" t="s">
@@ -4187,7 +4203,7 @@
       </c>
       <c r="R27" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="S27" s="23"/>
       <c r="T27" s="46" t="s">
@@ -4244,7 +4260,7 @@
       </c>
       <c r="R28" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="S28" s="23">
         <v>4066655983</v>
@@ -4305,7 +4321,7 @@
       </c>
       <c r="R29" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="S29" s="23"/>
       <c r="T29" s="23"/>
@@ -4362,7 +4378,7 @@
       </c>
       <c r="R30" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="S30" s="23" t="s">
         <v>119</v>
@@ -4428,7 +4444,7 @@
       </c>
       <c r="R31" s="31">
         <f t="shared" ref="R31" ca="1" si="7">IF(Q31="","",(TODAY()-Q31))</f>
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S31" s="23" t="s">
         <v>126</v>
@@ -4487,7 +4503,7 @@
       </c>
       <c r="R32" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="S32" s="23"/>
       <c r="T32" s="46" t="s">
@@ -4548,7 +4564,7 @@
       </c>
       <c r="R33" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="S33" s="23"/>
       <c r="T33" s="46" t="s">
@@ -4609,7 +4625,7 @@
       </c>
       <c r="R34" s="31">
         <f t="shared" ref="R34:R39" ca="1" si="9">IF(Q34="","",(TODAY()-Q34))</f>
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="S34" s="23" t="s">
         <v>139</v>
@@ -4672,7 +4688,7 @@
       </c>
       <c r="R35" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="S35" s="23"/>
       <c r="T35" s="46" t="s">
@@ -4733,7 +4749,7 @@
       </c>
       <c r="R36" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="S36" s="23" t="s">
         <v>148</v>
@@ -4796,7 +4812,7 @@
       </c>
       <c r="R37" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="S37" s="23" t="s">
         <v>153</v>
@@ -4859,7 +4875,7 @@
       </c>
       <c r="R38" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="S38" s="23" t="s">
         <v>157</v>
@@ -4920,7 +4936,7 @@
       </c>
       <c r="R39" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S39" s="23" t="s">
         <v>162</v>
@@ -4979,7 +4995,7 @@
       </c>
       <c r="R40" s="31">
         <f ca="1">IF(Q40="","",(TODAY()-Q40))</f>
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="S40" s="50" t="s">
         <v>165</v>
@@ -5043,7 +5059,7 @@
       </c>
       <c r="R41" s="131">
         <f t="shared" ref="R41:R50" ca="1" si="11">IF(Q41="","",(TODAY()-Q41))</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S41" s="129" t="s">
         <v>169</v>
@@ -5107,7 +5123,7 @@
       </c>
       <c r="R42" s="131">
         <f t="shared" ca="1" si="11"/>
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="S42" s="129"/>
       <c r="T42" s="134" t="s">
@@ -5146,7 +5162,7 @@
       <c r="I43" s="42"/>
       <c r="J43" s="41">
         <f t="shared" ca="1" si="10"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K43" s="41" t="s">
         <v>39</v>
@@ -5169,7 +5185,7 @@
       </c>
       <c r="R43" s="41">
         <f t="shared" ca="1" si="11"/>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S43" s="39" t="s">
         <v>162</v>
@@ -5200,7 +5216,7 @@
         <v>135</v>
       </c>
       <c r="G44" s="39" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="H44" s="42">
         <v>45995</v>
@@ -5208,7 +5224,7 @@
       <c r="I44" s="39"/>
       <c r="J44" s="41">
         <f t="shared" ca="1" si="10"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K44" s="41" t="s">
         <v>42</v>
@@ -5229,12 +5245,16 @@
       </c>
       <c r="R44" s="41">
         <f t="shared" ca="1" si="11"/>
-        <v>99</v>
-      </c>
-      <c r="S44" s="39"/>
-      <c r="T44" s="39"/>
+        <v>100</v>
+      </c>
+      <c r="S44" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="T44" s="136" t="s">
+        <v>222</v>
+      </c>
       <c r="U44" s="135" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.25">
@@ -5243,7 +5263,7 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C45" s="52"/>
       <c r="D45" s="1"/>
@@ -5263,7 +5283,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C46" s="52"/>
       <c r="D46" s="1"/>
@@ -5287,7 +5307,7 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C47" s="52"/>
       <c r="D47" s="1"/>
@@ -5307,7 +5327,7 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C48" s="52"/>
       <c r="D48" s="1"/>
@@ -5327,7 +5347,7 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" s="52"/>
       <c r="D49" s="1"/>
@@ -5347,7 +5367,7 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C50" s="52"/>
       <c r="D50" s="1"/>
@@ -5367,7 +5387,7 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" s="52"/>
       <c r="D51" s="1"/>
@@ -5383,7 +5403,7 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C52" s="52"/>
       <c r="D52" s="1"/>
@@ -5399,7 +5419,7 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C53" s="52"/>
       <c r="D53" s="1"/>
@@ -5415,7 +5435,7 @@
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C54" s="52"/>
       <c r="D54" s="1"/>
@@ -5431,7 +5451,7 @@
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C55" s="52"/>
       <c r="D55" s="1"/>
@@ -5447,7 +5467,7 @@
         <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C56" s="52"/>
       <c r="D56" s="1"/>
@@ -5463,7 +5483,7 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C57" s="52"/>
       <c r="D57" s="1"/>
@@ -5479,7 +5499,7 @@
         <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C58" s="52"/>
       <c r="D58" s="1"/>
@@ -5495,7 +5515,7 @@
         <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C59" s="52"/>
       <c r="D59" s="1"/>
@@ -5511,7 +5531,7 @@
         <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C60" s="52"/>
       <c r="D60" s="1"/>
@@ -5527,7 +5547,7 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C61" s="52"/>
       <c r="D61" s="1"/>
@@ -5543,7 +5563,7 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C62" s="52"/>
       <c r="D62" s="1"/>
@@ -5559,7 +5579,7 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C63" s="52"/>
       <c r="D63" s="1"/>
@@ -5575,7 +5595,7 @@
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C64" s="52"/>
       <c r="D64" s="1"/>
@@ -5591,7 +5611,7 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C65" s="52"/>
       <c r="D65" s="1"/>
@@ -5607,7 +5627,7 @@
         <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C66" s="52"/>
       <c r="D66" s="1"/>
@@ -5623,7 +5643,7 @@
         <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C67" s="52"/>
       <c r="D67" s="1"/>
@@ -5639,7 +5659,7 @@
         <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C68" s="52"/>
       <c r="D68" s="1"/>
@@ -5655,7 +5675,7 @@
         <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C69" s="52"/>
       <c r="D69" s="1"/>
@@ -5671,7 +5691,7 @@
         <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C70" s="52"/>
       <c r="D70" s="1"/>
@@ -5687,7 +5707,7 @@
         <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C71" s="52"/>
       <c r="D71" s="1"/>
@@ -5703,7 +5723,7 @@
         <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C72" s="52"/>
       <c r="D72" s="1"/>
@@ -5719,7 +5739,7 @@
         <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C73" s="52"/>
       <c r="D73" s="1"/>
@@ -5735,7 +5755,7 @@
         <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C74" s="52"/>
       <c r="D74" s="1"/>
@@ -5751,7 +5771,7 @@
         <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C75" s="52"/>
       <c r="D75" s="1"/>
@@ -5767,7 +5787,7 @@
         <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C76" s="52"/>
       <c r="D76" s="1"/>
@@ -5783,16 +5803,16 @@
         <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C77" s="52"/>
       <c r="D77" s="1"/>
       <c r="K77" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L77" s="53"/>
       <c r="M77" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N77">
         <f t="shared" si="12"/>
@@ -5805,7 +5825,7 @@
         <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C78" s="52"/>
       <c r="D78" s="1"/>
@@ -5821,7 +5841,7 @@
         <v>75</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C79" s="52"/>
       <c r="D79" s="1"/>
@@ -5837,7 +5857,7 @@
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C80" s="52"/>
       <c r="D80" s="1"/>
@@ -5853,7 +5873,7 @@
         <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C81" s="52"/>
       <c r="D81" s="1"/>
@@ -5868,7 +5888,7 @@
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C82" s="52"/>
       <c r="D82" s="1"/>
@@ -5883,7 +5903,7 @@
         <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C83" s="52"/>
       <c r="D83" s="1"/>
@@ -5898,7 +5918,7 @@
         <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C84" s="52"/>
       <c r="D84" s="1"/>
@@ -5913,7 +5933,7 @@
         <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C85" s="52"/>
       <c r="D85" s="1"/>
@@ -5928,7 +5948,7 @@
         <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C86" s="52"/>
       <c r="D86" s="1"/>
@@ -5943,7 +5963,7 @@
         <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C87" s="52"/>
       <c r="D87" s="1"/>
@@ -5958,7 +5978,7 @@
         <v>84</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C88" s="52"/>
       <c r="D88" s="1"/>
@@ -5973,7 +5993,7 @@
         <v>85</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C89" s="52"/>
       <c r="D89" s="1"/>
@@ -5988,7 +6008,7 @@
         <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C90" s="52"/>
       <c r="D90" s="1"/>
@@ -6003,7 +6023,7 @@
         <v>87</v>
       </c>
       <c r="B91" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C91" s="52"/>
       <c r="D91" s="1"/>
@@ -6018,7 +6038,7 @@
         <v>88</v>
       </c>
       <c r="B92" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C92" s="52"/>
       <c r="D92" s="1"/>
@@ -6033,7 +6053,7 @@
         <v>89</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C93" s="52"/>
       <c r="D93" s="1"/>
@@ -6048,7 +6068,7 @@
         <v>90</v>
       </c>
       <c r="B94" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C94" s="52"/>
       <c r="D94" s="1"/>
@@ -6063,7 +6083,7 @@
         <v>91</v>
       </c>
       <c r="B95" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C95" s="52"/>
       <c r="D95" s="1"/>
@@ -6078,7 +6098,7 @@
         <v>92</v>
       </c>
       <c r="B96" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C96" s="52"/>
       <c r="D96" s="1"/>
@@ -6093,7 +6113,7 @@
         <v>93</v>
       </c>
       <c r="B97" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C97" s="52"/>
       <c r="D97" s="1"/>
@@ -6108,7 +6128,7 @@
         <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C98" s="52"/>
       <c r="D98" s="1"/>
@@ -6123,7 +6143,7 @@
         <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C99" s="52"/>
       <c r="D99" s="1"/>
@@ -6138,7 +6158,7 @@
         <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C100" s="52"/>
       <c r="D100" s="1"/>
@@ -6153,7 +6173,7 @@
         <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C101" s="52"/>
       <c r="D101" s="1"/>
@@ -6168,7 +6188,7 @@
         <v>98</v>
       </c>
       <c r="B102" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C102" s="52"/>
       <c r="D102" s="1"/>
@@ -6178,28 +6198,28 @@
       </c>
     </row>
     <row r="104" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="141" t="s">
-        <v>178</v>
-      </c>
-      <c r="B104" s="142"/>
-      <c r="C104" s="142"/>
-      <c r="D104" s="142"/>
-      <c r="E104" s="142"/>
-      <c r="F104" s="142"/>
-      <c r="G104" s="142"/>
-      <c r="H104" s="142"/>
-      <c r="I104" s="142"/>
-      <c r="J104" s="142"/>
-      <c r="K104" s="142"/>
-      <c r="L104" s="142"/>
-      <c r="M104" s="142"/>
-      <c r="N104" s="142"/>
-      <c r="O104" s="142"/>
-      <c r="P104" s="142"/>
-      <c r="Q104" s="142"/>
-      <c r="R104" s="142"/>
-      <c r="S104" s="142"/>
-      <c r="T104" s="142"/>
+      <c r="A104" s="142" t="s">
+        <v>177</v>
+      </c>
+      <c r="B104" s="143"/>
+      <c r="C104" s="143"/>
+      <c r="D104" s="143"/>
+      <c r="E104" s="143"/>
+      <c r="F104" s="143"/>
+      <c r="G104" s="143"/>
+      <c r="H104" s="143"/>
+      <c r="I104" s="143"/>
+      <c r="J104" s="143"/>
+      <c r="K104" s="143"/>
+      <c r="L104" s="143"/>
+      <c r="M104" s="143"/>
+      <c r="N104" s="143"/>
+      <c r="O104" s="143"/>
+      <c r="P104" s="143"/>
+      <c r="Q104" s="143"/>
+      <c r="R104" s="143"/>
+      <c r="S104" s="143"/>
+      <c r="T104" s="143"/>
     </row>
     <row r="105" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="54"/>
@@ -6228,7 +6248,7 @@
         <v>30</v>
       </c>
       <c r="C106" s="56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D106">
         <v>4</v>
@@ -6240,7 +6260,7 @@
         <v>64</v>
       </c>
       <c r="G106" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P106" s="57">
         <v>22019</v>
@@ -6249,7 +6269,7 @@
         <v>6266167273</v>
       </c>
       <c r="T106" s="58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U106">
         <v>1289</v>
@@ -6263,7 +6283,7 @@
         <v>30</v>
       </c>
       <c r="C107" s="56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D107">
         <v>4</v>
@@ -6272,19 +6292,19 @@
         <v>31</v>
       </c>
       <c r="F107" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G107" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P107" s="57">
         <v>21789</v>
       </c>
       <c r="S107" t="s">
+        <v>183</v>
+      </c>
+      <c r="T107" s="58" t="s">
         <v>184</v>
-      </c>
-      <c r="T107" s="58" t="s">
-        <v>185</v>
       </c>
       <c r="U107">
         <v>2737</v>
@@ -6486,6 +6506,7 @@
     <hyperlink ref="T42" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="T106" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="T107" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="T44" r:id="rId18" xr:uid="{0599F4F2-3FEC-471D-91C0-22E677C933D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="90" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -6528,41 +6549,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
-      <c r="P1" s="144"/>
-      <c r="Q1" s="144"/>
-      <c r="R1" s="144"/>
-      <c r="S1" s="144"/>
+      <c r="A1" s="144" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
+      <c r="R1" s="145"/>
+      <c r="S1" s="145"/>
       <c r="T1" s="59"/>
     </row>
     <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="138">
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="139">
         <f ca="1">(TODAY())</f>
-        <v>46061</v>
-      </c>
-      <c r="F2" s="138"/>
+        <v>46062</v>
+      </c>
+      <c r="F2" s="139"/>
       <c r="G2" s="61" t="s">
         <v>2</v>
       </c>
@@ -6574,11 +6595,11 @@
         <f>N2+P2</f>
         <v>5</v>
       </c>
-      <c r="K2" s="145" t="s">
+      <c r="K2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="145"/>
-      <c r="M2" s="145"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
       <c r="N2" s="63">
         <f>COUNTIF(D4:D14, "M")</f>
         <v>5</v>
@@ -6591,7 +6612,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R2" s="66">
         <f>COUNTIF(L4:L17, "H")</f>
@@ -6604,7 +6625,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" s="69"/>
       <c r="D3" s="69" t="s">
@@ -6620,7 +6641,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I3" s="70" t="s">
         <v>17</v>
@@ -6629,7 +6650,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="68" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L3" s="70" t="s">
         <v>20</v>
@@ -6653,7 +6674,7 @@
         <v>26</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T3" s="59"/>
     </row>
@@ -6699,14 +6720,14 @@
       <c r="H5" s="74"/>
       <c r="I5" s="6">
         <f t="shared" ref="I5:I6" ca="1" si="0">IF(G5="","",IF(H5="",TODAY()-G5,DATEDIF(G5,H5,"d")))</f>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K5" s="53"/>
       <c r="L5" s="75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M5" s="74"/>
       <c r="N5" s="1"/>
@@ -6718,7 +6739,7 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" ref="Q5:Q6" ca="1" si="1">IF(P5="","",(TODAY()-P5))</f>
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>84</v>
@@ -6741,7 +6762,7 @@
         <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="57">
         <v>45891</v>
@@ -6749,7 +6770,7 @@
       <c r="H6" s="74"/>
       <c r="I6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>33</v>
@@ -6758,7 +6779,7 @@
         <v>87</v>
       </c>
       <c r="L6" s="75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M6" s="74"/>
       <c r="N6" s="1"/>
@@ -6767,7 +6788,7 @@
       </c>
       <c r="Q6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="R6" s="1"/>
       <c r="T6" s="59"/>
@@ -6777,7 +6798,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" s="76"/>
       <c r="D7" s="77" t="s">
@@ -6794,13 +6815,13 @@
       </c>
       <c r="I7" s="1">
         <f ca="1">IF(G7="","",IF(H7="",TODAY()-G7,DATEDIF(G7,H7,"d")))</f>
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>46</v>
       </c>
       <c r="K7" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>138</v>
@@ -6814,7 +6835,7 @@
       </c>
       <c r="Q7" s="1">
         <f t="shared" ref="Q7:Q8" ca="1" si="3">IF(P7="","",(TODAY()-P7))</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R7" s="76" t="s">
         <v>169</v>
@@ -6830,7 +6851,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="76" t="s">
         <v>36</v>
@@ -6846,13 +6867,13 @@
       </c>
       <c r="I8" s="6">
         <f ca="1">IF(G8="","",IF(H8="",TODAY()-G8,DATEDIF(G8,H8,"d")))</f>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="K8" s="53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>138</v>
@@ -6869,7 +6890,7 @@
       </c>
       <c r="Q8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="S8" s="58" t="s">
         <v>174</v>
@@ -6882,7 +6903,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" s="52">
         <v>135</v>
@@ -6902,7 +6923,7 @@
       <c r="H9" s="57"/>
       <c r="I9" s="1">
         <f t="shared" ref="I9" ca="1" si="5">IF(G9="","",IF(H9="",TODAY()-G9,DATEDIF(G9,H9,"d")))</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>39</v>
@@ -6925,7 +6946,7 @@
       </c>
       <c r="Q9" s="1">
         <f t="shared" ref="Q9" ca="1" si="6">IF(P9="","",(TODAY()-P9))</f>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R9" t="s">
         <v>162</v>
@@ -7021,11 +7042,11 @@
     </row>
     <row r="20" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E20" t="str">
         <f t="array" aca="1" ref="E20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
-        <v>James</v>
+        <v>Naftali</v>
       </c>
       <c r="F20">
         <f t="array" aca="1" ref="F20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
@@ -7104,31 +7125,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="86"/>
-      <c r="B1" s="170" t="s">
-        <v>200</v>
-      </c>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
+      <c r="B1" s="147" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="148"/>
       <c r="I1" s="86"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="86"/>
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="149" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="150"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="152" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="175" t="s">
-        <v>202</v>
-      </c>
-      <c r="G2" s="176"/>
-      <c r="H2" s="177"/>
-      <c r="I2" s="178"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="155"/>
     </row>
     <row r="3" spans="1:9" ht="5.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="86"/>
@@ -7139,23 +7160,23 @@
       <c r="F3" s="91"/>
       <c r="G3" s="92"/>
       <c r="H3" s="93"/>
-      <c r="I3" s="178"/>
+      <c r="I3" s="155"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="86"/>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="156" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="95" t="s">
         <v>203</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>204</v>
       </c>
       <c r="D4" s="96"/>
       <c r="E4" s="86"/>
-      <c r="F4" s="165" t="s">
-        <v>205</v>
+      <c r="F4" s="159" t="s">
+        <v>204</v>
       </c>
       <c r="G4" s="97" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H4" s="98" t="s">
         <v>86</v>
@@ -7164,15 +7185,15 @@
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
-      <c r="B5" s="153"/>
+      <c r="B5" s="157"/>
       <c r="C5" s="99" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" s="100"/>
       <c r="E5" s="86"/>
-      <c r="F5" s="166"/>
+      <c r="F5" s="160"/>
       <c r="G5" s="101" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H5" s="102" t="s">
         <v>172</v>
@@ -7181,49 +7202,49 @@
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="86"/>
-      <c r="B6" s="154"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6" s="104"/>
       <c r="E6" s="86"/>
-      <c r="F6" s="167"/>
+      <c r="F6" s="161"/>
       <c r="G6" s="103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H6" s="105"/>
       <c r="I6" s="86"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="86"/>
-      <c r="B7" s="152" t="s">
-        <v>208</v>
+      <c r="B7" s="156" t="s">
+        <v>207</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" s="106"/>
       <c r="E7" s="86"/>
-      <c r="F7" s="165" t="s">
-        <v>209</v>
+      <c r="F7" s="159" t="s">
+        <v>208</v>
       </c>
       <c r="G7" s="97" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H7" s="98"/>
       <c r="I7" s="86"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="86"/>
-      <c r="B8" s="153"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="99" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8" s="107"/>
       <c r="E8" s="86"/>
-      <c r="F8" s="166"/>
+      <c r="F8" s="160"/>
       <c r="G8" s="101" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H8" s="102" t="s">
         <v>81</v>
@@ -7232,66 +7253,66 @@
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="86"/>
-      <c r="B9" s="154"/>
+      <c r="B9" s="158"/>
       <c r="C9" s="103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="105"/>
       <c r="E9" s="86"/>
-      <c r="F9" s="167"/>
+      <c r="F9" s="161"/>
       <c r="G9" s="103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H9" s="105"/>
       <c r="I9" s="86"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="86"/>
-      <c r="B10" s="152" t="s">
-        <v>210</v>
+      <c r="B10" s="156" t="s">
+        <v>209</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="106"/>
       <c r="E10" s="86"/>
-      <c r="F10" s="168" t="s">
-        <v>211</v>
+      <c r="F10" s="162" t="s">
+        <v>210</v>
       </c>
       <c r="G10" s="108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H10" s="109"/>
       <c r="I10" s="86"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="86"/>
-      <c r="B11" s="153"/>
+      <c r="B11" s="157"/>
       <c r="C11" s="99" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" s="107"/>
       <c r="E11" s="86"/>
-      <c r="F11" s="169"/>
+      <c r="F11" s="163"/>
       <c r="G11" s="110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H11" s="111"/>
       <c r="I11" s="86"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="86"/>
-      <c r="B12" s="154"/>
+      <c r="B12" s="158"/>
       <c r="C12" s="112" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="113"/>
       <c r="E12" s="86"/>
-      <c r="F12" s="168" t="s">
-        <v>212</v>
+      <c r="F12" s="162" t="s">
+        <v>211</v>
       </c>
       <c r="G12" s="97" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H12" s="92" t="s">
         <v>159</v>
@@ -7301,85 +7322,85 @@
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="86"/>
       <c r="B13" s="94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C13" s="95" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="106"/>
       <c r="E13" s="86"/>
-      <c r="F13" s="169"/>
+      <c r="F13" s="163"/>
       <c r="G13" s="101" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H13" s="102" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I13" s="86"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="86"/>
-      <c r="B14" s="152" t="s">
-        <v>215</v>
+      <c r="B14" s="156" t="s">
+        <v>214</v>
       </c>
       <c r="C14" s="114" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D14" s="115"/>
       <c r="E14" s="86"/>
       <c r="F14" s="116"/>
       <c r="G14" s="103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H14" s="105"/>
       <c r="I14" s="86"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="86"/>
-      <c r="B15" s="153"/>
+      <c r="B15" s="157"/>
       <c r="C15" s="117" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="118"/>
       <c r="E15" s="86"/>
-      <c r="F15" s="155"/>
+      <c r="F15" s="164"/>
       <c r="G15" s="114"/>
       <c r="H15" s="115"/>
       <c r="I15" s="86"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="86"/>
-      <c r="B16" s="154"/>
+      <c r="B16" s="158"/>
       <c r="C16" s="103" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" s="105"/>
       <c r="E16" s="86"/>
-      <c r="F16" s="156"/>
+      <c r="F16" s="165"/>
       <c r="G16" s="117"/>
       <c r="H16" s="118"/>
       <c r="I16" s="86"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="86"/>
-      <c r="B17" s="158" t="s">
-        <v>216</v>
+      <c r="B17" s="167" t="s">
+        <v>215</v>
       </c>
       <c r="C17" s="114" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="115"/>
       <c r="E17" s="86"/>
-      <c r="F17" s="157"/>
+      <c r="F17" s="166"/>
       <c r="G17" s="103"/>
       <c r="H17" s="105"/>
       <c r="I17" s="86"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="86"/>
-      <c r="B18" s="159"/>
+      <c r="B18" s="168"/>
       <c r="C18" s="117" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D18" s="118"/>
       <c r="E18" s="86"/>
@@ -7400,90 +7421,90 @@
       <c r="I19" s="86"/>
     </row>
     <row r="20" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="160" t="s">
-        <v>217</v>
-      </c>
-      <c r="B20" s="160"/>
-      <c r="C20" s="160"/>
-      <c r="D20" s="160"/>
-      <c r="E20" s="160"/>
-      <c r="F20" s="160"/>
-      <c r="G20" s="160"/>
-      <c r="H20" s="160"/>
-      <c r="I20" s="160"/>
+      <c r="A20" s="169" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" s="169"/>
+      <c r="C20" s="169"/>
+      <c r="D20" s="169"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="169"/>
+      <c r="H20" s="169"/>
+      <c r="I20" s="169"/>
     </row>
     <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="160"/>
-      <c r="B21" s="160"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="160"/>
-      <c r="E21" s="160"/>
-      <c r="F21" s="160"/>
-      <c r="G21" s="160"/>
-      <c r="H21" s="160"/>
-      <c r="I21" s="160"/>
+      <c r="A21" s="169"/>
+      <c r="B21" s="169"/>
+      <c r="C21" s="169"/>
+      <c r="D21" s="169"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="169"/>
+      <c r="H21" s="169"/>
+      <c r="I21" s="169"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="86"/>
       <c r="B22" s="122" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" s="170" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="161" t="s">
-        <v>219</v>
-      </c>
-      <c r="D22" s="162"/>
+      <c r="D22" s="171"/>
       <c r="E22" s="123"/>
       <c r="F22" s="124" t="s">
+        <v>217</v>
+      </c>
+      <c r="G22" s="172" t="s">
         <v>218</v>
       </c>
-      <c r="G22" s="163" t="s">
-        <v>219</v>
-      </c>
-      <c r="H22" s="164"/>
+      <c r="H22" s="173"/>
       <c r="I22" s="86"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="86"/>
       <c r="B23" s="125"/>
-      <c r="C23" s="149"/>
-      <c r="D23" s="149"/>
+      <c r="C23" s="177"/>
+      <c r="D23" s="177"/>
       <c r="E23" s="86"/>
       <c r="F23" s="126"/>
-      <c r="G23" s="150"/>
-      <c r="H23" s="151"/>
+      <c r="G23" s="178"/>
+      <c r="H23" s="179"/>
       <c r="I23" s="86"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="86"/>
       <c r="B24" s="127"/>
-      <c r="C24" s="146"/>
-      <c r="D24" s="146"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="174"/>
       <c r="E24" s="86"/>
       <c r="F24" s="128"/>
-      <c r="G24" s="147"/>
-      <c r="H24" s="148"/>
+      <c r="G24" s="175"/>
+      <c r="H24" s="176"/>
       <c r="I24" s="86"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="86"/>
       <c r="B25" s="127"/>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
+      <c r="C25" s="174"/>
+      <c r="D25" s="174"/>
       <c r="E25" s="86"/>
       <c r="F25" s="128"/>
-      <c r="G25" s="147"/>
-      <c r="H25" s="148"/>
+      <c r="G25" s="175"/>
+      <c r="H25" s="176"/>
       <c r="I25" s="86"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="86"/>
       <c r="B26" s="127"/>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146"/>
+      <c r="C26" s="174"/>
+      <c r="D26" s="174"/>
       <c r="E26" s="86"/>
       <c r="F26" s="128"/>
-      <c r="G26" s="147"/>
-      <c r="H26" s="148"/>
+      <c r="G26" s="175"/>
+      <c r="H26" s="176"/>
       <c r="I26" s="86"/>
     </row>
     <row r="27" spans="1:9" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
@@ -7499,23 +7520,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A20:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="C23:D23"/>
@@ -7524,6 +7528,23 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="F4:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add print header and signature to member-agreement intake form
</commit_message>
<xml_diff>
--- a/members .xlsx
+++ b/members .xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29725"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{B7497AC0-A7B1-4A41-910A-4EC7CFA4F027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F83A87B5-DE5D-4532-8D43-C6C7C932678B}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{B7497AC0-A7B1-4A41-910A-4EC7CFA4F027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114282C1-AC5F-4DFD-8790-0C3F534C3897}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43905" yWindow="2325" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="225">
   <si>
     <t>HORIZON-HOUSE MASTER LIST</t>
   </si>
@@ -758,6 +758,12 @@
   </si>
   <si>
     <t>ryantokeski5@gmail.com</t>
+  </si>
+  <si>
+    <t>bk 7</t>
+  </si>
+  <si>
+    <t>500+</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1799,6 +1805,78 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1826,84 +1904,271 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="6"/>
@@ -2389,10 +2654,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2712,34 +2973,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1796875" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="12" width="6.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="1" customWidth="1"/>
+    <col min="11" max="12" width="6.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.54296875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.54296875" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="1" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
-    <col min="20" max="20" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" customWidth="1"/>
+    <col min="18" max="18" width="7.453125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.54296875" customWidth="1"/>
+    <col min="20" max="20" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="137" t="s">
         <v>0</v>
@@ -2763,7 +3024,7 @@
       <c r="S1" s="137"/>
       <c r="T1" s="137"/>
     </row>
-    <row r="2" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="138" t="s">
         <v>1</v>
       </c>
@@ -2772,7 +3033,7 @@
       <c r="E2" s="138"/>
       <c r="F2" s="139">
         <f ca="1">(TODAY())</f>
-        <v>46062</v>
+        <v>46067</v>
       </c>
       <c r="G2" s="139"/>
       <c r="H2" s="3"/>
@@ -2782,7 +3043,7 @@
       </c>
       <c r="K2" s="5">
         <f>O2+Q2</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
@@ -2798,7 +3059,7 @@
       </c>
       <c r="Q2" s="10">
         <f>COUNTIF(E5:E202,"F")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>5</v>
@@ -2807,7 +3068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="140" t="s">
         <v>7</v>
       </c>
@@ -2828,7 +3089,7 @@
       <c r="Q3" s="10"/>
       <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="1:22" s="12" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="12" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -2896,7 +3157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2924,7 +3185,7 @@
       </c>
       <c r="J5" s="25">
         <f ca="1">(TODAY()-H5)</f>
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>33</v>
@@ -2948,7 +3209,7 @@
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
     </row>
-    <row r="6" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <f>A5+1</f>
         <v>2</v>
@@ -3003,12 +3264,12 @@
       </c>
       <c r="R6" s="31">
         <f ca="1">IF(Q6="","",(TODAY()-Q6))</f>
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
     </row>
-    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A70" si="0">A6+1</f>
         <v>3</v>
@@ -3060,7 +3321,7 @@
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
     </row>
-    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3112,7 +3373,7 @@
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
     </row>
-    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3165,14 +3426,14 @@
       </c>
       <c r="R9" s="31">
         <f ca="1">IF(Q9="","",(TODAY()-Q9))</f>
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="S9" s="23"/>
       <c r="T9" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3227,12 +3488,12 @@
       </c>
       <c r="R10" s="31">
         <f t="shared" ref="R10:R33" ca="1" si="4">IF(Q10="","",(TODAY()-Q10))</f>
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
     </row>
-    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3290,7 +3551,7 @@
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
     </row>
-    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3343,7 +3604,7 @@
       <c r="S12" s="23"/>
       <c r="T12" s="23"/>
     </row>
-    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3396,12 +3657,12 @@
       </c>
       <c r="R13" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
     </row>
-    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3454,12 +3715,12 @@
       </c>
       <c r="R14" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
     </row>
-    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3512,14 +3773,14 @@
       </c>
       <c r="R15" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="S15" s="23" t="s">
         <v>65</v>
       </c>
       <c r="T15" s="23"/>
     </row>
-    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3572,14 +3833,14 @@
       </c>
       <c r="R16" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="S16" s="23" t="s">
         <v>70</v>
       </c>
       <c r="T16" s="23"/>
     </row>
-    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3631,7 +3892,7 @@
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
     </row>
-    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3683,7 +3944,7 @@
       <c r="S18" s="23"/>
       <c r="T18" s="23"/>
     </row>
-    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3736,14 +3997,14 @@
       </c>
       <c r="R19" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="S19" s="23" t="s">
         <v>79</v>
       </c>
       <c r="T19" s="23"/>
     </row>
-    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3773,7 +4034,7 @@
       <c r="I20" s="39"/>
       <c r="J20" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="K20" s="41" t="s">
         <v>50</v>
@@ -3794,7 +4055,7 @@
       </c>
       <c r="R20" s="41">
         <f t="shared" ca="1" si="4"/>
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="S20" s="39" t="s">
         <v>84</v>
@@ -3804,7 +4065,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3855,12 +4116,12 @@
       </c>
       <c r="R21" s="25">
         <f t="shared" ca="1" si="4"/>
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
     </row>
-    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3912,12 +4173,12 @@
       </c>
       <c r="R22" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="S22" s="23"/>
       <c r="T22" s="23"/>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3971,14 +4232,14 @@
       </c>
       <c r="R23" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="S23" s="23"/>
       <c r="T23" s="46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4028,7 +4289,7 @@
       </c>
       <c r="R24" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="S24" s="23" t="s">
         <v>99</v>
@@ -4037,7 +4298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4087,7 +4348,7 @@
       </c>
       <c r="R25" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="S25" s="23" t="s">
         <v>103</v>
@@ -4096,7 +4357,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4146,14 +4407,14 @@
       </c>
       <c r="R26" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="S26" s="23"/>
       <c r="T26" s="46" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4203,14 +4464,14 @@
       </c>
       <c r="R27" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="S27" s="23"/>
       <c r="T27" s="46" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4260,7 +4521,7 @@
       </c>
       <c r="R28" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="S28" s="23">
         <v>4066655983</v>
@@ -4269,7 +4530,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4321,12 +4582,12 @@
       </c>
       <c r="R29" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="S29" s="23"/>
       <c r="T29" s="23"/>
     </row>
-    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4378,7 +4639,7 @@
       </c>
       <c r="R30" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="S30" s="23" t="s">
         <v>119</v>
@@ -4390,7 +4651,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4444,7 +4705,7 @@
       </c>
       <c r="R31" s="31">
         <f t="shared" ref="R31" ca="1" si="7">IF(Q31="","",(TODAY()-Q31))</f>
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="S31" s="23" t="s">
         <v>126</v>
@@ -4453,7 +4714,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4503,14 +4764,14 @@
       </c>
       <c r="R32" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="S32" s="23"/>
       <c r="T32" s="46" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4564,14 +4825,14 @@
       </c>
       <c r="R33" s="31">
         <f t="shared" ca="1" si="4"/>
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="S33" s="23"/>
       <c r="T33" s="46" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4625,7 +4886,7 @@
       </c>
       <c r="R34" s="31">
         <f t="shared" ref="R34:R39" ca="1" si="9">IF(Q34="","",(TODAY()-Q34))</f>
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="S34" s="23" t="s">
         <v>139</v>
@@ -4634,7 +4895,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4688,14 +4949,14 @@
       </c>
       <c r="R35" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="S35" s="23"/>
       <c r="T35" s="46" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4749,7 +5010,7 @@
       </c>
       <c r="R36" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="S36" s="23" t="s">
         <v>148</v>
@@ -4758,7 +5019,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4812,7 +5073,7 @@
       </c>
       <c r="R37" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="S37" s="23" t="s">
         <v>153</v>
@@ -4821,7 +5082,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4875,14 +5136,14 @@
       </c>
       <c r="R38" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="S38" s="23" t="s">
         <v>157</v>
       </c>
       <c r="T38" s="23"/>
     </row>
-    <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4936,14 +5197,14 @@
       </c>
       <c r="R39" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="S39" s="23" t="s">
         <v>162</v>
       </c>
       <c r="T39" s="23"/>
     </row>
-    <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4995,7 +5256,7 @@
       </c>
       <c r="R40" s="31">
         <f ca="1">IF(Q40="","",(TODAY()-Q40))</f>
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="S40" s="50" t="s">
         <v>165</v>
@@ -5007,7 +5268,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -5037,7 +5298,7 @@
         <v>46033</v>
       </c>
       <c r="J41" s="131">
-        <f t="shared" ref="J41:J44" ca="1" si="10">IF(H41="","",IF(I41="",TODAY()-H41,DATEDIF(H41,I41,"d")))</f>
+        <f t="shared" ref="J41:J45" ca="1" si="10">IF(H41="","",IF(I41="",TODAY()-H41,DATEDIF(H41,I41,"d")))</f>
         <v>97</v>
       </c>
       <c r="K41" s="131" t="s">
@@ -5059,7 +5320,7 @@
       </c>
       <c r="R41" s="131">
         <f t="shared" ref="R41:R50" ca="1" si="11">IF(Q41="","",(TODAY()-Q41))</f>
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="S41" s="129" t="s">
         <v>169</v>
@@ -5071,7 +5332,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -5123,7 +5384,7 @@
       </c>
       <c r="R42" s="131">
         <f t="shared" ca="1" si="11"/>
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="S42" s="129"/>
       <c r="T42" s="134" t="s">
@@ -5133,7 +5394,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5162,7 +5423,7 @@
       <c r="I43" s="42"/>
       <c r="J43" s="41">
         <f t="shared" ca="1" si="10"/>
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="K43" s="41" t="s">
         <v>39</v>
@@ -5185,7 +5446,7 @@
       </c>
       <c r="R43" s="41">
         <f t="shared" ca="1" si="11"/>
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="S43" s="39" t="s">
         <v>162</v>
@@ -5195,7 +5456,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -5224,7 +5485,7 @@
       <c r="I44" s="39"/>
       <c r="J44" s="41">
         <f t="shared" ca="1" si="10"/>
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K44" s="41" t="s">
         <v>42</v>
@@ -5245,7 +5506,7 @@
       </c>
       <c r="R44" s="41">
         <f t="shared" ca="1" si="11"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S44" s="39" t="s">
         <v>221</v>
@@ -5257,7 +5518,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -5265,19 +5526,60 @@
       <c r="B45" t="s">
         <v>175</v>
       </c>
-      <c r="C45" s="52"/>
-      <c r="D45" s="1"/>
-      <c r="L45" s="53"/>
-      <c r="N45">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R45" s="1" t="str">
+      <c r="C45" s="52">
+        <v>141</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="180" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H45" s="33">
+        <v>46066</v>
+      </c>
+      <c r="I45" s="33"/>
+      <c r="J45" s="37">
+        <f t="shared" ca="1" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="K45" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="L45" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="M45" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="N45" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="O45" s="23"/>
+      <c r="P45" s="33">
+        <v>28391</v>
+      </c>
+      <c r="Q45" s="33">
+        <v>45848</v>
+      </c>
+      <c r="R45" s="31">
         <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="S45" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T45" s="46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -5301,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -5321,7 +5623,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -5341,7 +5643,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5361,7 +5663,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -5381,7 +5683,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5397,7 +5699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5413,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -5429,7 +5731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -5445,7 +5747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -5461,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -5477,7 +5779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -5493,7 +5795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -5509,7 +5811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -5525,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -5541,7 +5843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -5557,7 +5859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -5573,7 +5875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -5589,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -5605,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -5621,7 +5923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -5637,7 +5939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -5653,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -5669,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -5685,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -5701,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <f t="shared" ref="A71:A102" si="13">A70+1</f>
         <v>67</v>
@@ -5717,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <f t="shared" si="13"/>
         <v>68</v>
@@ -5733,7 +6035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <f t="shared" si="13"/>
         <v>69</v>
@@ -5749,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <f t="shared" si="13"/>
         <v>70</v>
@@ -5765,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <f t="shared" si="13"/>
         <v>71</v>
@@ -5781,7 +6083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <f t="shared" si="13"/>
         <v>72</v>
@@ -5797,7 +6099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <f t="shared" si="13"/>
         <v>73</v>
@@ -5819,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <f t="shared" si="13"/>
         <v>74</v>
@@ -5835,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <f t="shared" si="13"/>
         <v>75</v>
@@ -5851,7 +6153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <f t="shared" si="13"/>
         <v>76</v>
@@ -5867,7 +6169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <f t="shared" si="13"/>
         <v>77</v>
@@ -5882,7 +6184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <f t="shared" si="13"/>
         <v>78</v>
@@ -5897,7 +6199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <f t="shared" si="13"/>
         <v>79</v>
@@ -5912,7 +6214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <f t="shared" si="13"/>
         <v>80</v>
@@ -5927,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <f t="shared" si="13"/>
         <v>81</v>
@@ -5942,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <f t="shared" si="13"/>
         <v>82</v>
@@ -5957,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <f t="shared" si="13"/>
         <v>83</v>
@@ -5972,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <f t="shared" si="13"/>
         <v>84</v>
@@ -5987,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <f t="shared" si="13"/>
         <v>85</v>
@@ -6002,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <f t="shared" si="13"/>
         <v>86</v>
@@ -6017,7 +6319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <f t="shared" si="13"/>
         <v>87</v>
@@ -6032,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <f t="shared" si="13"/>
         <v>88</v>
@@ -6047,7 +6349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <f t="shared" si="13"/>
         <v>89</v>
@@ -6062,7 +6364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <f t="shared" si="13"/>
         <v>90</v>
@@ -6077,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <f t="shared" si="13"/>
         <v>91</v>
@@ -6092,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <f t="shared" si="13"/>
         <v>92</v>
@@ -6107,7 +6409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <f t="shared" si="13"/>
         <v>93</v>
@@ -6122,7 +6424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <f t="shared" si="13"/>
         <v>94</v>
@@ -6137,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <f t="shared" si="13"/>
         <v>95</v>
@@ -6152,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <f t="shared" si="13"/>
         <v>96</v>
@@ -6167,7 +6469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <f t="shared" si="13"/>
         <v>97</v>
@@ -6182,7 +6484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <f t="shared" si="13"/>
         <v>98</v>
@@ -6197,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A104" s="142" t="s">
         <v>177</v>
       </c>
@@ -6221,7 +6523,7 @@
       <c r="S104" s="143"/>
       <c r="T104" s="143"/>
     </row>
-    <row r="105" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A105" s="54"/>
       <c r="B105" s="55"/>
       <c r="C105" s="55"/>
@@ -6243,7 +6545,7 @@
       <c r="S105" s="55"/>
       <c r="T105" s="55"/>
     </row>
-    <row r="106" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>30</v>
       </c>
@@ -6278,7 +6580,7 @@
         <v>128934</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>30</v>
       </c>
@@ -6313,28 +6615,28 @@
         <v>273727</v>
       </c>
     </row>
-    <row r="108" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C108" s="56"/>
     </row>
-    <row r="109" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C109" s="56"/>
     </row>
-    <row r="110" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C110" s="56"/>
     </row>
-    <row r="111" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C111" s="56"/>
     </row>
-    <row r="112" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C112" s="56"/>
     </row>
-    <row r="113" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" s="56"/>
     </row>
-    <row r="114" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114" s="56"/>
     </row>
-    <row r="115" spans="3:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115" s="56"/>
     </row>
   </sheetData>
@@ -6346,146 +6648,178 @@
     <mergeCell ref="A104:T104"/>
   </mergeCells>
   <conditionalFormatting sqref="R21">
-    <cfRule type="cellIs" dxfId="43" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="39" operator="between">
       <formula>91</formula>
       <formula>179</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="38" operator="between">
       <formula>1</formula>
       <formula>29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="40" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="41" operator="between">
       <formula>61</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="42" operator="equal">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="43" operator="equal">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="60" priority="44" operator="between">
       <formula>31</formula>
       <formula>59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29:R30">
-    <cfRule type="cellIs" dxfId="35" priority="55" operator="between">
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="between">
       <formula>91</formula>
       <formula>119</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="57" operator="between">
+    <cfRule type="cellIs" dxfId="58" priority="65" operator="between">
       <formula>61</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="60" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="68" operator="between">
       <formula>31</formula>
       <formula>59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29:R31">
-    <cfRule type="cellIs" dxfId="32" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="46" operator="between">
+    <cfRule type="cellIs" dxfId="55" priority="54" operator="between">
       <formula>1</formula>
       <formula>29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="59" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R31">
-    <cfRule type="cellIs" dxfId="27" priority="47" operator="between">
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="between">
       <formula>91</formula>
       <formula>179</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="49" operator="between">
+    <cfRule type="cellIs" dxfId="50" priority="57" operator="between">
       <formula>61</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="52" operator="between">
+    <cfRule type="cellIs" dxfId="49" priority="60" operator="between">
       <formula>31</formula>
       <formula>59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R36">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
       <formula>60</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R37">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="44" priority="20" operator="between">
       <formula>31</formula>
       <formula>59</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="43" priority="17" operator="between">
       <formula>1</formula>
       <formula>29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="between">
       <formula>91</formula>
       <formula>179</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="19" operator="between">
       <formula>61</formula>
       <formula>89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R40">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="between">
       <formula>1</formula>
       <formula>29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="between">
       <formula>91</formula>
       <formula>179</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="between">
       <formula>61</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="equal">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="15" operator="equal">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="between">
       <formula>31</formula>
       <formula>59</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5">
-    <cfRule type="expression" dxfId="8" priority="63">
+    <cfRule type="expression" dxfId="32" priority="71">
       <formula>"G4&lt;0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R45">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>90</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R45">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>1</formula>
+      <formula>29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>91</formula>
+      <formula>179</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+      <formula>61</formula>
+      <formula>89</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
+      <formula>31</formula>
+      <formula>59</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -6507,6 +6841,7 @@
     <hyperlink ref="T106" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="T107" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="T44" r:id="rId18" xr:uid="{0599F4F2-3FEC-471D-91C0-22E677C933D5}"/>
+    <hyperlink ref="T45" r:id="rId19" xr:uid="{4566973C-6CC0-4D2E-9BF3-545EE3E877C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="90" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -6524,31 +6859,31 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="3" max="3" width="0.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" customWidth="1"/>
+    <col min="3" max="3" width="0.7265625" customWidth="1"/>
+    <col min="4" max="4" width="3.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="0.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="0.7265625" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
     <col min="13" max="13" width="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="5.85546875" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" customWidth="1"/>
-    <col min="19" max="19" width="29.5703125" customWidth="1"/>
-    <col min="20" max="20" width="34.7109375" customWidth="1"/>
+    <col min="14" max="14" width="7.54296875" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" customWidth="1"/>
+    <col min="17" max="17" width="5.81640625" customWidth="1"/>
+    <col min="18" max="18" width="13.54296875" customWidth="1"/>
+    <col min="19" max="19" width="29.54296875" customWidth="1"/>
+    <col min="20" max="20" width="34.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="144" t="s">
         <v>185</v>
       </c>
@@ -6572,7 +6907,7 @@
       <c r="S1" s="145"/>
       <c r="T1" s="59"/>
     </row>
-    <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60"/>
       <c r="B2" s="138" t="s">
         <v>1</v>
@@ -6581,7 +6916,7 @@
       <c r="D2" s="138"/>
       <c r="E2" s="139">
         <f ca="1">(TODAY())</f>
-        <v>46062</v>
+        <v>46067</v>
       </c>
       <c r="F2" s="139"/>
       <c r="G2" s="61" t="s">
@@ -6620,7 +6955,7 @@
       </c>
       <c r="T2" s="59"/>
     </row>
-    <row r="3" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="67" t="s">
         <v>8</v>
       </c>
@@ -6678,7 +7013,7 @@
       </c>
       <c r="T3" s="59"/>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="73"/>
       <c r="C4" s="52"/>
       <c r="D4" s="1"/>
@@ -6696,7 +7031,7 @@
       <c r="R4" s="1"/>
       <c r="T4" s="59"/>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="73">
         <f>A4+1</f>
         <v>1</v>
@@ -6720,7 +7055,7 @@
       <c r="H5" s="74"/>
       <c r="I5" s="6">
         <f t="shared" ref="I5:I6" ca="1" si="0">IF(G5="","",IF(H5="",TODAY()-G5,DATEDIF(G5,H5,"d")))</f>
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>50</v>
@@ -6739,14 +7074,14 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" ref="Q5:Q6" ca="1" si="1">IF(P5="","",(TODAY()-P5))</f>
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>84</v>
       </c>
       <c r="T5" s="59"/>
     </row>
-    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="73">
         <f t="shared" ref="A6" si="2">A5+1</f>
         <v>2</v>
@@ -6770,7 +7105,7 @@
       <c r="H6" s="74"/>
       <c r="I6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>33</v>
@@ -6788,12 +7123,12 @@
       </c>
       <c r="Q6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="R6" s="1"/>
       <c r="T6" s="59"/>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="73">
         <v>3</v>
       </c>
@@ -6815,7 +7150,7 @@
       </c>
       <c r="I7" s="1">
         <f ca="1">IF(G7="","",IF(H7="",TODAY()-G7,DATEDIF(G7,H7,"d")))</f>
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>46</v>
@@ -6835,7 +7170,7 @@
       </c>
       <c r="Q7" s="1">
         <f t="shared" ref="Q7:Q8" ca="1" si="3">IF(P7="","",(TODAY()-P7))</f>
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="R7" s="76" t="s">
         <v>169</v>
@@ -6845,7 +7180,7 @@
       </c>
       <c r="T7" s="59"/>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="73">
         <f t="shared" ref="A8:A13" si="4">A7+1</f>
         <v>4</v>
@@ -6867,7 +7202,7 @@
       </c>
       <c r="I8" s="6">
         <f ca="1">IF(G8="","",IF(H8="",TODAY()-G8,DATEDIF(G8,H8,"d")))</f>
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>75</v>
@@ -6890,14 +7225,14 @@
       </c>
       <c r="Q8" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="S8" s="58" t="s">
         <v>174</v>
       </c>
       <c r="T8" s="59"/>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="73">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -6923,7 +7258,7 @@
       <c r="H9" s="57"/>
       <c r="I9" s="1">
         <f t="shared" ref="I9" ca="1" si="5">IF(G9="","",IF(H9="",TODAY()-G9,DATEDIF(G9,H9,"d")))</f>
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>39</v>
@@ -6946,35 +7281,35 @@
       </c>
       <c r="Q9" s="1">
         <f t="shared" ref="Q9" ca="1" si="6">IF(P9="","",(TODAY()-P9))</f>
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="R9" t="s">
         <v>162</v>
       </c>
       <c r="T9" s="59"/>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="73">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="T10" s="59"/>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="73">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="T11" s="59"/>
     </row>
-    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="73">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="T12" s="59"/>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="73">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -6990,13 +7325,13 @@
       <c r="S13" s="58"/>
       <c r="T13" s="59"/>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="78">
         <v>14</v>
       </c>
       <c r="T14" s="59"/>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="79"/>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
@@ -7022,39 +7357,39 @@
       <c r="S15" s="79"/>
       <c r="T15" s="59"/>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K16" s="56"/>
       <c r="L16" s="85"/>
       <c r="M16" s="74"/>
     </row>
-    <row r="17" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="K17" s="56"/>
       <c r="L17" s="76"/>
     </row>
-    <row r="18" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="57"/>
       <c r="K18" s="56"/>
     </row>
-    <row r="19" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="F19" s="57"/>
       <c r="G19" s="57"/>
       <c r="K19" s="56"/>
     </row>
-    <row r="20" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>198</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E20">
         <f t="array" aca="1" ref="E20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
+        <v>0</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="array" aca="1" ref="F20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
         <v>Naftali</v>
       </c>
-      <c r="F20">
-        <f t="array" aca="1" ref="F20" ca="1">INDEX(E4:E14, RANDBETWEEN(1, COUNTA(E4:E14)))</f>
-        <v>0</v>
-      </c>
       <c r="K20" s="56"/>
     </row>
-    <row r="21" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="K21" s="56"/>
     </row>
   </sheetData>
@@ -7065,31 +7400,31 @@
     <mergeCell ref="K2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="Q4:Q6 Q13">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="between">
       <formula>1</formula>
       <formula>29</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="between">
       <formula>91</formula>
       <formula>179</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="between">
       <formula>61</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="between">
       <formula>31</formula>
       <formula>59</formula>
     </cfRule>
@@ -7111,47 +7446,47 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="1.54296875" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" customWidth="1"/>
+    <col min="3" max="3" width="2.54296875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="3.453125" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="9" max="9" width="1.42578125" customWidth="1"/>
+    <col min="9" max="9" width="1.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="86"/>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="171" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
       <c r="I1" s="86"/>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="86"/>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="173" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="151"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="175"/>
       <c r="E2" s="87"/>
-      <c r="F2" s="152" t="s">
+      <c r="F2" s="176" t="s">
         <v>201</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="155"/>
-    </row>
-    <row r="3" spans="1:9" ht="5.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="177"/>
+      <c r="H2" s="178"/>
+      <c r="I2" s="179"/>
+    </row>
+    <row r="3" spans="1:9" ht="5.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="86"/>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -7160,11 +7495,11 @@
       <c r="F3" s="91"/>
       <c r="G3" s="92"/>
       <c r="H3" s="93"/>
-      <c r="I3" s="155"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="I3" s="179"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="86"/>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="153" t="s">
         <v>202</v>
       </c>
       <c r="C4" s="95" t="s">
@@ -7172,7 +7507,7 @@
       </c>
       <c r="D4" s="96"/>
       <c r="E4" s="86"/>
-      <c r="F4" s="159" t="s">
+      <c r="F4" s="166" t="s">
         <v>204</v>
       </c>
       <c r="G4" s="97" t="s">
@@ -7183,15 +7518,15 @@
       </c>
       <c r="I4" s="86"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="86"/>
-      <c r="B5" s="157"/>
+      <c r="B5" s="154"/>
       <c r="C5" s="99" t="s">
         <v>205</v>
       </c>
       <c r="D5" s="100"/>
       <c r="E5" s="86"/>
-      <c r="F5" s="160"/>
+      <c r="F5" s="167"/>
       <c r="G5" s="101" t="s">
         <v>205</v>
       </c>
@@ -7200,24 +7535,24 @@
       </c>
       <c r="I5" s="86"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="86"/>
-      <c r="B6" s="158"/>
+      <c r="B6" s="155"/>
       <c r="C6" s="103" t="s">
         <v>206</v>
       </c>
       <c r="D6" s="104"/>
       <c r="E6" s="86"/>
-      <c r="F6" s="161"/>
+      <c r="F6" s="168"/>
       <c r="G6" s="103" t="s">
         <v>206</v>
       </c>
       <c r="H6" s="105"/>
       <c r="I6" s="86"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="86"/>
-      <c r="B7" s="156" t="s">
+      <c r="B7" s="153" t="s">
         <v>207</v>
       </c>
       <c r="C7" s="95" t="s">
@@ -7225,7 +7560,7 @@
       </c>
       <c r="D7" s="106"/>
       <c r="E7" s="86"/>
-      <c r="F7" s="159" t="s">
+      <c r="F7" s="166" t="s">
         <v>208</v>
       </c>
       <c r="G7" s="97" t="s">
@@ -7234,15 +7569,15 @@
       <c r="H7" s="98"/>
       <c r="I7" s="86"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="86"/>
-      <c r="B8" s="157"/>
+      <c r="B8" s="154"/>
       <c r="C8" s="99" t="s">
         <v>205</v>
       </c>
       <c r="D8" s="107"/>
       <c r="E8" s="86"/>
-      <c r="F8" s="160"/>
+      <c r="F8" s="167"/>
       <c r="G8" s="101" t="s">
         <v>205</v>
       </c>
@@ -7251,24 +7586,24 @@
       </c>
       <c r="I8" s="86"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="86"/>
-      <c r="B9" s="158"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="103" t="s">
         <v>206</v>
       </c>
       <c r="D9" s="105"/>
       <c r="E9" s="86"/>
-      <c r="F9" s="161"/>
+      <c r="F9" s="168"/>
       <c r="G9" s="103" t="s">
         <v>206</v>
       </c>
       <c r="H9" s="105"/>
       <c r="I9" s="86"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="86"/>
-      <c r="B10" s="156" t="s">
+      <c r="B10" s="153" t="s">
         <v>209</v>
       </c>
       <c r="C10" s="95" t="s">
@@ -7276,7 +7611,7 @@
       </c>
       <c r="D10" s="106"/>
       <c r="E10" s="86"/>
-      <c r="F10" s="162" t="s">
+      <c r="F10" s="169" t="s">
         <v>210</v>
       </c>
       <c r="G10" s="108" t="s">
@@ -7285,30 +7620,30 @@
       <c r="H10" s="109"/>
       <c r="I10" s="86"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="86"/>
-      <c r="B11" s="157"/>
+      <c r="B11" s="154"/>
       <c r="C11" s="99" t="s">
         <v>205</v>
       </c>
       <c r="D11" s="107"/>
       <c r="E11" s="86"/>
-      <c r="F11" s="163"/>
+      <c r="F11" s="170"/>
       <c r="G11" s="110" t="s">
         <v>205</v>
       </c>
       <c r="H11" s="111"/>
       <c r="I11" s="86"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="86"/>
-      <c r="B12" s="158"/>
+      <c r="B12" s="155"/>
       <c r="C12" s="112" t="s">
         <v>206</v>
       </c>
       <c r="D12" s="113"/>
       <c r="E12" s="86"/>
-      <c r="F12" s="162" t="s">
+      <c r="F12" s="169" t="s">
         <v>211</v>
       </c>
       <c r="G12" s="97" t="s">
@@ -7319,7 +7654,7 @@
       </c>
       <c r="I12" s="86"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="86"/>
       <c r="B13" s="94" t="s">
         <v>212</v>
@@ -7329,7 +7664,7 @@
       </c>
       <c r="D13" s="106"/>
       <c r="E13" s="86"/>
-      <c r="F13" s="163"/>
+      <c r="F13" s="170"/>
       <c r="G13" s="101" t="s">
         <v>205</v>
       </c>
@@ -7338,9 +7673,9 @@
       </c>
       <c r="I13" s="86"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="86"/>
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="153" t="s">
         <v>214</v>
       </c>
       <c r="C14" s="114" t="s">
@@ -7355,35 +7690,35 @@
       <c r="H14" s="105"/>
       <c r="I14" s="86"/>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="86"/>
-      <c r="B15" s="157"/>
+      <c r="B15" s="154"/>
       <c r="C15" s="117" t="s">
         <v>205</v>
       </c>
       <c r="D15" s="118"/>
       <c r="E15" s="86"/>
-      <c r="F15" s="164"/>
+      <c r="F15" s="156"/>
       <c r="G15" s="114"/>
       <c r="H15" s="115"/>
       <c r="I15" s="86"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="86"/>
-      <c r="B16" s="158"/>
+      <c r="B16" s="155"/>
       <c r="C16" s="103" t="s">
         <v>206</v>
       </c>
       <c r="D16" s="105"/>
       <c r="E16" s="86"/>
-      <c r="F16" s="165"/>
+      <c r="F16" s="157"/>
       <c r="G16" s="117"/>
       <c r="H16" s="118"/>
       <c r="I16" s="86"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="86"/>
-      <c r="B17" s="167" t="s">
+      <c r="B17" s="159" t="s">
         <v>215</v>
       </c>
       <c r="C17" s="114" t="s">
@@ -7391,14 +7726,14 @@
       </c>
       <c r="D17" s="115"/>
       <c r="E17" s="86"/>
-      <c r="F17" s="166"/>
+      <c r="F17" s="158"/>
       <c r="G17" s="103"/>
       <c r="H17" s="105"/>
       <c r="I17" s="86"/>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="86"/>
-      <c r="B18" s="168"/>
+      <c r="B18" s="160"/>
       <c r="C18" s="117" t="s">
         <v>205</v>
       </c>
@@ -7409,7 +7744,7 @@
       <c r="H18" s="121"/>
       <c r="I18" s="86"/>
     </row>
-    <row r="19" spans="1:9" ht="9.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="9.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="86"/>
       <c r="B19" s="86"/>
       <c r="C19" s="86"/>
@@ -7420,94 +7755,94 @@
       <c r="H19" s="86"/>
       <c r="I19" s="86"/>
     </row>
-    <row r="20" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="169" t="s">
+    <row r="20" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="161" t="s">
         <v>216</v>
       </c>
-      <c r="B20" s="169"/>
-      <c r="C20" s="169"/>
-      <c r="D20" s="169"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="169"/>
-    </row>
-    <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="169"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
-      <c r="F21" s="169"/>
-      <c r="G21" s="169"/>
-      <c r="H21" s="169"/>
-      <c r="I21" s="169"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="161"/>
+      <c r="C20" s="161"/>
+      <c r="D20" s="161"/>
+      <c r="E20" s="161"/>
+      <c r="F20" s="161"/>
+      <c r="G20" s="161"/>
+      <c r="H20" s="161"/>
+      <c r="I20" s="161"/>
+    </row>
+    <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="161"/>
+      <c r="B21" s="161"/>
+      <c r="C21" s="161"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="161"/>
+      <c r="F21" s="161"/>
+      <c r="G21" s="161"/>
+      <c r="H21" s="161"/>
+      <c r="I21" s="161"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="86"/>
       <c r="B22" s="122" t="s">
         <v>217</v>
       </c>
-      <c r="C22" s="170" t="s">
+      <c r="C22" s="162" t="s">
         <v>218</v>
       </c>
-      <c r="D22" s="171"/>
+      <c r="D22" s="163"/>
       <c r="E22" s="123"/>
       <c r="F22" s="124" t="s">
         <v>217</v>
       </c>
-      <c r="G22" s="172" t="s">
+      <c r="G22" s="164" t="s">
         <v>218</v>
       </c>
-      <c r="H22" s="173"/>
+      <c r="H22" s="165"/>
       <c r="I22" s="86"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="86"/>
       <c r="B23" s="125"/>
-      <c r="C23" s="177"/>
-      <c r="D23" s="177"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="150"/>
       <c r="E23" s="86"/>
       <c r="F23" s="126"/>
-      <c r="G23" s="178"/>
-      <c r="H23" s="179"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="152"/>
       <c r="I23" s="86"/>
     </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="86"/>
       <c r="B24" s="127"/>
-      <c r="C24" s="174"/>
-      <c r="D24" s="174"/>
+      <c r="C24" s="147"/>
+      <c r="D24" s="147"/>
       <c r="E24" s="86"/>
       <c r="F24" s="128"/>
-      <c r="G24" s="175"/>
-      <c r="H24" s="176"/>
+      <c r="G24" s="148"/>
+      <c r="H24" s="149"/>
       <c r="I24" s="86"/>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="86"/>
       <c r="B25" s="127"/>
-      <c r="C25" s="174"/>
-      <c r="D25" s="174"/>
+      <c r="C25" s="147"/>
+      <c r="D25" s="147"/>
       <c r="E25" s="86"/>
       <c r="F25" s="128"/>
-      <c r="G25" s="175"/>
-      <c r="H25" s="176"/>
+      <c r="G25" s="148"/>
+      <c r="H25" s="149"/>
       <c r="I25" s="86"/>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="86"/>
       <c r="B26" s="127"/>
-      <c r="C26" s="174"/>
-      <c r="D26" s="174"/>
+      <c r="C26" s="147"/>
+      <c r="D26" s="147"/>
       <c r="E26" s="86"/>
       <c r="F26" s="128"/>
-      <c r="G26" s="175"/>
-      <c r="H26" s="176"/>
+      <c r="G26" s="148"/>
+      <c r="H26" s="149"/>
       <c r="I26" s="86"/>
     </row>
-    <row r="27" spans="1:9" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="86"/>
       <c r="B27" s="86"/>
       <c r="C27" s="86"/>
@@ -7520,6 +7855,23 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="C23:D23"/>
@@ -7528,23 +7880,6 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A20:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="F4:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>